<commit_message>
okno serwisowe - aktualizacja
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -1049,7 +1049,7 @@
     <t>17.2.a Official development assistance as a proportion of gross national income</t>
   </si>
   <si>
-    <t>Last update: 22-12-2020, 14:19</t>
+    <t>Last update: 12-01-2021, 12:01</t>
   </si>
 </sst>
 </file>
@@ -1592,8 +1592,8 @@
   <dimension ref="A1:R175"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
okno serwisowe pdf, excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -1049,7 +1049,7 @@
     <t>17.2.a Official development assistance as a proportion of gross national income</t>
   </si>
   <si>
-    <t>Last update: 12-01-2021, 12:01</t>
+    <t>Last update: 26-01-2021, 12:46</t>
   </si>
 </sst>
 </file>
@@ -1592,7 +1592,7 @@
   <dimension ref="A1:R175"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -8083,25 +8083,25 @@
       </c>
       <c r="G130" s="3"/>
       <c r="H130" s="6">
-        <v>120451</v>
+        <v>10166</v>
       </c>
       <c r="I130" s="6">
-        <v>-63307</v>
+        <v>-27471</v>
       </c>
       <c r="J130" s="6">
-        <v>63845</v>
+        <v>11803</v>
       </c>
       <c r="K130" s="6">
-        <v>295265</v>
+        <v>35266</v>
       </c>
       <c r="L130" s="6">
-        <v>250661</v>
+        <v>24986</v>
       </c>
       <c r="M130" s="6">
-        <v>433179</v>
+        <v>49727</v>
       </c>
       <c r="N130" s="6">
-        <v>1127454</v>
+        <v>46034</v>
       </c>
       <c r="O130" s="3"/>
       <c r="P130" s="3"/>
@@ -10363,7 +10363,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="66" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe - 02.02.2021
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="342">
   <si>
     <t>sdg.gov.pl/en</t>
   </si>
@@ -573,7 +573,7 @@
     <t>7.3.a Relation of energy acquisition in general to the global energy consumption</t>
   </si>
   <si>
-    <t>Ministry of Energy / Statistics Poland</t>
+    <t>Ministry of Climate and Environment / Statistics Poland</t>
   </si>
   <si>
     <t>7.3.b SAIDI (System Average Interruption Duration Index)</t>
@@ -725,7 +725,7 @@
     <t>9.2.b Business enterprise expenditure on R&amp;D in relation to GDP</t>
   </si>
   <si>
-    <t>9.2.c Share of net revenues from sales of new or significantly improved products in total turnover in industrial enterprises</t>
+    <t>9.2.c Share of net revenues from sales of new or improved products in total turnover in industrial enterprises</t>
   </si>
   <si>
     <t>9.2.d Share of export of high technology products in total export</t>
@@ -761,12 +761,16 @@
     <t>Goal 10. Reduce inequalities</t>
   </si>
   <si>
+    <t>Overcoming of regional socio-economic disparities, prevention of new
+  development disproportions</t>
+  </si>
+  <si>
+    <t>10.1.a Differentiation of gross value added per person employed in total at regional level (NUTS 2)</t>
+  </si>
+  <si>
     <t>Overcoming of regional socio-economic disparities, prevention of new development disproportions</t>
   </si>
   <si>
-    <t>10.1.a Differentiation of gross value added per person employed in total at regional level (NUTS 2)</t>
-  </si>
-  <si>
     <t>10.1.b Average annual net disposable income per capita in a household in rural areas in relation to urban areas</t>
   </si>
   <si>
@@ -1049,7 +1053,7 @@
     <t>17.2.a Official development assistance as a proportion of gross national income</t>
   </si>
   <si>
-    <t>Last update: 26-01-2021, 12:46</t>
+    <t>Last update: 02-02-2021, 09:09</t>
   </si>
 </sst>
 </file>
@@ -1856,33 +1860,35 @@
         <v>30</v>
       </c>
       <c r="G7" s="5">
-        <v>107.05</v>
+        <v>107.56</v>
       </c>
       <c r="H7" s="5">
-        <v>107.44</v>
+        <v>107.93</v>
       </c>
       <c r="I7" s="5">
-        <v>108.58</v>
+        <v>108.78</v>
       </c>
       <c r="J7" s="5">
-        <v>110.19</v>
+        <v>110.25</v>
       </c>
       <c r="K7" s="5">
-        <v>113.39</v>
+        <v>113.67</v>
       </c>
       <c r="L7" s="5">
-        <v>117.66</v>
+        <v>118.48</v>
       </c>
       <c r="M7" s="5">
-        <v>124.68</v>
+        <v>125.18</v>
       </c>
       <c r="N7" s="5">
-        <v>128.55000000000001</v>
+        <v>129.18</v>
       </c>
       <c r="O7" s="5">
-        <v>132.25</v>
-      </c>
-      <c r="P7" s="3"/>
+        <v>133.29</v>
+      </c>
+      <c r="P7" s="5">
+        <v>141.4</v>
+      </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="2" t="s">
         <v>25</v>
@@ -1978,7 +1984,9 @@
       <c r="O9" s="4">
         <v>116.1</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="4">
+        <v>115.4</v>
+      </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="2" t="s">
         <v>25</v>
@@ -2188,7 +2196,9 @@
       <c r="O13" s="5">
         <v>0.05</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="5">
+        <v>0.06</v>
+      </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="2" t="s">
         <v>25</v>
@@ -2615,7 +2625,9 @@
       <c r="P21" s="6">
         <v>85876</v>
       </c>
-      <c r="Q21" s="3"/>
+      <c r="Q21" s="6">
+        <v>85876</v>
+      </c>
       <c r="R21" s="2" t="s">
         <v>65</v>
       </c>
@@ -2669,7 +2681,9 @@
       <c r="P22" s="6">
         <v>4453</v>
       </c>
-      <c r="Q22" s="3"/>
+      <c r="Q22" s="6">
+        <v>4350</v>
+      </c>
       <c r="R22" s="2" t="s">
         <v>65</v>
       </c>
@@ -2723,7 +2737,9 @@
       <c r="P23" s="6">
         <v>1497</v>
       </c>
-      <c r="Q23" s="3"/>
+      <c r="Q23" s="6">
+        <v>1578</v>
+      </c>
       <c r="R23" s="2" t="s">
         <v>65</v>
       </c>
@@ -2777,7 +2793,9 @@
       <c r="P24" s="6">
         <v>8198</v>
       </c>
-      <c r="Q24" s="3"/>
+      <c r="Q24" s="6">
+        <v>8160</v>
+      </c>
       <c r="R24" s="2" t="s">
         <v>65</v>
       </c>
@@ -2831,7 +2849,9 @@
       <c r="P25" s="6">
         <v>144</v>
       </c>
-      <c r="Q25" s="3"/>
+      <c r="Q25" s="6">
+        <v>156</v>
+      </c>
       <c r="R25" s="2" t="s">
         <v>65</v>
       </c>
@@ -2885,7 +2905,9 @@
       <c r="P26" s="6">
         <v>37589</v>
       </c>
-      <c r="Q26" s="3"/>
+      <c r="Q26" s="6">
+        <v>40100</v>
+      </c>
       <c r="R26" s="2" t="s">
         <v>65</v>
       </c>
@@ -3440,7 +3462,9 @@
       <c r="O37" s="4">
         <v>23.3</v>
       </c>
-      <c r="P37" s="3"/>
+      <c r="P37" s="4">
+        <v>23.7</v>
+      </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="2" t="s">
         <v>25</v>
@@ -3492,7 +3516,9 @@
       <c r="O38" s="4">
         <v>56.2</v>
       </c>
-      <c r="P38" s="3"/>
+      <c r="P38" s="4">
+        <v>56.3</v>
+      </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="2" t="s">
         <v>25</v>
@@ -4392,7 +4418,9 @@
       <c r="O58" s="4">
         <v>87.3</v>
       </c>
-      <c r="P58" s="3"/>
+      <c r="P58" s="4">
+        <v>88.5</v>
+      </c>
       <c r="Q58" s="3"/>
       <c r="R58" s="2" t="s">
         <v>131</v>
@@ -4444,7 +4472,9 @@
       <c r="O59" s="4">
         <v>101.9</v>
       </c>
-      <c r="P59" s="3"/>
+      <c r="P59" s="4">
+        <v>102.7</v>
+      </c>
       <c r="Q59" s="3"/>
       <c r="R59" s="2" t="s">
         <v>131</v>
@@ -4496,7 +4526,9 @@
       <c r="O60" s="4">
         <v>67</v>
       </c>
-      <c r="P60" s="3"/>
+      <c r="P60" s="4">
+        <v>68.5</v>
+      </c>
       <c r="Q60" s="3"/>
       <c r="R60" s="2" t="s">
         <v>131</v>
@@ -5065,7 +5097,9 @@
       <c r="P71" s="6">
         <v>21</v>
       </c>
-      <c r="Q71" s="3"/>
+      <c r="Q71" s="6">
+        <v>26</v>
+      </c>
       <c r="R71" s="2" t="s">
         <v>25</v>
       </c>
@@ -5108,7 +5142,7 @@
         <v>7.4</v>
       </c>
       <c r="M72" s="4">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="N72" s="4">
         <v>7.2</v>
@@ -5116,10 +5150,12 @@
       <c r="O72" s="4">
         <v>8.8000000000000007</v>
       </c>
-      <c r="P72" s="3"/>
+      <c r="P72" s="4">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="Q72" s="3"/>
       <c r="R72" s="2" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -5876,39 +5912,41 @@
         <v>24</v>
       </c>
       <c r="G88" s="5">
-        <v>9.25</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H88" s="5">
-        <v>10.29</v>
+        <v>10.35</v>
       </c>
       <c r="I88" s="5">
-        <v>10.9</v>
+        <v>10.97</v>
       </c>
       <c r="J88" s="5">
-        <v>11.37</v>
+        <v>11.46</v>
       </c>
       <c r="K88" s="5">
-        <v>11.5</v>
+        <v>11.61</v>
       </c>
       <c r="L88" s="5">
-        <v>11.74</v>
+        <v>11.89</v>
       </c>
       <c r="M88" s="5">
-        <v>11.27</v>
+        <v>11.4</v>
       </c>
       <c r="N88" s="5">
-        <v>10.96</v>
+        <v>11.12</v>
       </c>
       <c r="O88" s="5">
-        <v>11.28</v>
-      </c>
-      <c r="P88" s="3"/>
+        <v>11.48</v>
+      </c>
+      <c r="P88" s="5">
+        <v>12.16</v>
+      </c>
       <c r="Q88" s="3"/>
       <c r="R88" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>174</v>
       </c>
@@ -5954,7 +5992,9 @@
       <c r="O89" s="6">
         <v>58</v>
       </c>
-      <c r="P89" s="3"/>
+      <c r="P89" s="6">
+        <v>57</v>
+      </c>
       <c r="Q89" s="3"/>
       <c r="R89" s="2" t="s">
         <v>182</v>
@@ -6321,7 +6361,9 @@
       <c r="P96" s="6">
         <v>40</v>
       </c>
-      <c r="Q96" s="3"/>
+      <c r="Q96" s="6">
+        <v>40</v>
+      </c>
       <c r="R96" s="2" t="s">
         <v>200</v>
       </c>
@@ -6912,7 +6954,9 @@
       <c r="O107" s="4">
         <v>73.900000000000006</v>
       </c>
-      <c r="P107" s="3"/>
+      <c r="P107" s="4">
+        <v>74.2</v>
+      </c>
       <c r="Q107" s="3"/>
       <c r="R107" s="2" t="s">
         <v>25</v>
@@ -7583,7 +7627,7 @@
         <v>0.88</v>
       </c>
       <c r="J120" s="5">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="K120" s="5">
         <v>0.94</v>
@@ -7600,7 +7644,9 @@
       <c r="O120" s="5">
         <v>1.21</v>
       </c>
-      <c r="P120" s="3"/>
+      <c r="P120" s="5">
+        <v>1.32</v>
+      </c>
       <c r="Q120" s="3"/>
       <c r="R120" s="2" t="s">
         <v>25</v>
@@ -7652,7 +7698,9 @@
       <c r="O121" s="5">
         <v>0.8</v>
       </c>
-      <c r="P121" s="3"/>
+      <c r="P121" s="5">
+        <v>0.83</v>
+      </c>
       <c r="Q121" s="3"/>
       <c r="R121" s="2" t="s">
         <v>25</v>
@@ -7704,7 +7752,9 @@
       <c r="O122" s="4">
         <v>9.1</v>
       </c>
-      <c r="P122" s="3"/>
+      <c r="P122" s="4">
+        <v>9.3000000000000007</v>
+      </c>
       <c r="Q122" s="3"/>
       <c r="R122" s="2" t="s">
         <v>25</v>
@@ -7968,7 +8018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>243</v>
       </c>
@@ -7987,24 +8037,36 @@
       <c r="F128" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G128" s="3"/>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="3"/>
+      <c r="G128" s="4">
+        <v>16.2</v>
+      </c>
+      <c r="H128" s="4">
+        <v>16.2</v>
+      </c>
+      <c r="I128" s="4">
+        <v>16</v>
+      </c>
+      <c r="J128" s="4">
+        <v>15.7</v>
+      </c>
       <c r="K128" s="4">
-        <v>16</v>
+        <v>15.7</v>
       </c>
       <c r="L128" s="4">
-        <v>15.7</v>
+        <v>15.5</v>
       </c>
       <c r="M128" s="4">
-        <v>15.2</v>
+        <v>15</v>
       </c>
       <c r="N128" s="4">
-        <v>14.8</v>
-      </c>
-      <c r="O128" s="3"/>
-      <c r="P128" s="3"/>
+        <v>14.7</v>
+      </c>
+      <c r="O128" s="4">
+        <v>15</v>
+      </c>
+      <c r="P128" s="4">
+        <v>15</v>
+      </c>
       <c r="Q128" s="3"/>
       <c r="R128" s="2" t="s">
         <v>25</v>
@@ -8015,10 +8077,10 @@
         <v>243</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>29</v>
@@ -8054,9 +8116,11 @@
         <v>68.900000000000006</v>
       </c>
       <c r="O129" s="4">
-        <v>77.8</v>
-      </c>
-      <c r="P129" s="3"/>
+        <v>71.7</v>
+      </c>
+      <c r="P129" s="4">
+        <v>77.099999999999994</v>
+      </c>
       <c r="Q129" s="3"/>
       <c r="R129" s="2" t="s">
         <v>25</v>
@@ -8067,10 +8131,10 @@
         <v>243</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>29</v>
@@ -8115,10 +8179,10 @@
         <v>243</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>29</v>
@@ -8127,7 +8191,7 @@
         <v>23</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G131" s="4">
         <v>31.1</v>
@@ -8156,7 +8220,9 @@
       <c r="O131" s="4">
         <v>27.8</v>
       </c>
-      <c r="P131" s="3"/>
+      <c r="P131" s="4">
+        <v>28.5</v>
+      </c>
       <c r="Q131" s="3"/>
       <c r="R131" s="2" t="s">
         <v>25</v>
@@ -8164,13 +8230,13 @@
     </row>
     <row r="132" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>29</v>
@@ -8208,7 +8274,9 @@
       <c r="O132" s="4">
         <v>13.8</v>
       </c>
-      <c r="P132" s="3"/>
+      <c r="P132" s="4">
+        <v>12.6</v>
+      </c>
       <c r="Q132" s="3"/>
       <c r="R132" s="2" t="s">
         <v>25</v>
@@ -8216,13 +8284,13 @@
     </row>
     <row r="133" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>29</v>
@@ -8270,13 +8338,13 @@
     </row>
     <row r="134" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>29</v>
@@ -8314,7 +8382,9 @@
       <c r="O134" s="4">
         <v>10.5</v>
       </c>
-      <c r="P134" s="3"/>
+      <c r="P134" s="4">
+        <v>10.4</v>
+      </c>
       <c r="Q134" s="3"/>
       <c r="R134" s="2" t="s">
         <v>25</v>
@@ -8322,13 +8392,13 @@
     </row>
     <row r="135" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>29</v>
@@ -8376,13 +8446,13 @@
     </row>
     <row r="136" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>29</v>
@@ -8425,24 +8495,24 @@
       </c>
       <c r="Q136" s="3"/>
       <c r="R136" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F137" s="3" t="s">
         <v>24</v>
@@ -8484,19 +8554,19 @@
     </row>
     <row r="138" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>24</v>
@@ -8538,19 +8608,19 @@
     </row>
     <row r="139" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>24</v>
@@ -8592,19 +8662,19 @@
     </row>
     <row r="140" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F140" s="3" t="s">
         <v>24</v>
@@ -8646,13 +8716,13 @@
     </row>
     <row r="141" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>29</v>
@@ -8700,13 +8770,13 @@
     </row>
     <row r="142" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>29</v>
@@ -8715,7 +8785,7 @@
         <v>23</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G142" s="4">
         <v>20.8</v>
@@ -8754,13 +8824,13 @@
     </row>
     <row r="143" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>29</v>
@@ -8769,7 +8839,7 @@
         <v>23</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G143" s="5">
         <v>0.56000000000000005</v>
@@ -8796,9 +8866,11 @@
         <v>0.64</v>
       </c>
       <c r="O143" s="5">
-        <v>0.62</v>
-      </c>
-      <c r="P143" s="3"/>
+        <v>0.65</v>
+      </c>
+      <c r="P143" s="5">
+        <v>0.71</v>
+      </c>
       <c r="Q143" s="3"/>
       <c r="R143" s="2" t="s">
         <v>83</v>
@@ -8806,13 +8878,13 @@
     </row>
     <row r="144" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>29</v>
@@ -8821,7 +8893,7 @@
         <v>23</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G144" s="5">
         <v>16.95</v>
@@ -8845,12 +8917,14 @@
         <v>17.7</v>
       </c>
       <c r="N144" s="5">
-        <v>18.760000000000002</v>
+        <v>18.71</v>
       </c>
       <c r="O144" s="5">
-        <v>20.37</v>
-      </c>
-      <c r="P144" s="3"/>
+        <v>19.34</v>
+      </c>
+      <c r="P144" s="5">
+        <v>18.489999999999998</v>
+      </c>
       <c r="Q144" s="3"/>
       <c r="R144" s="2" t="s">
         <v>83</v>
@@ -8858,13 +8932,13 @@
     </row>
     <row r="145" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>29</v>
@@ -8897,10 +8971,14 @@
         <v>10.199999999999999</v>
       </c>
       <c r="N145" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="O145" s="3"/>
-      <c r="P145" s="3"/>
+        <v>9.9</v>
+      </c>
+      <c r="O145" s="4">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="P145" s="4">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="Q145" s="3"/>
       <c r="R145" s="2" t="s">
         <v>83</v>
@@ -8908,13 +8986,13 @@
     </row>
     <row r="146" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>29</v>
@@ -8962,13 +9040,13 @@
     </row>
     <row r="147" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>29</v>
@@ -8977,7 +9055,7 @@
         <v>23</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G147" s="4">
         <v>100</v>
@@ -9009,18 +9087,18 @@
       <c r="P147" s="3"/>
       <c r="Q147" s="3"/>
       <c r="R147" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>29</v>
@@ -9029,7 +9107,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G148" s="4">
         <v>100</v>
@@ -9061,18 +9139,18 @@
       <c r="P148" s="3"/>
       <c r="Q148" s="3"/>
       <c r="R148" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>29</v>
@@ -9084,33 +9162,35 @@
         <v>24</v>
       </c>
       <c r="G149" s="5">
-        <v>9.25</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H149" s="5">
-        <v>10.29</v>
+        <v>10.35</v>
       </c>
       <c r="I149" s="5">
-        <v>10.9</v>
+        <v>10.97</v>
       </c>
       <c r="J149" s="5">
-        <v>11.37</v>
+        <v>11.46</v>
       </c>
       <c r="K149" s="5">
-        <v>11.5</v>
+        <v>11.61</v>
       </c>
       <c r="L149" s="5">
-        <v>11.74</v>
+        <v>11.89</v>
       </c>
       <c r="M149" s="5">
-        <v>11.27</v>
+        <v>11.4</v>
       </c>
       <c r="N149" s="5">
-        <v>10.96</v>
+        <v>11.12</v>
       </c>
       <c r="O149" s="5">
-        <v>11.28</v>
-      </c>
-      <c r="P149" s="3"/>
+        <v>11.48</v>
+      </c>
+      <c r="P149" s="5">
+        <v>12.16</v>
+      </c>
       <c r="Q149" s="3"/>
       <c r="R149" s="2" t="s">
         <v>25</v>
@@ -9118,13 +9198,13 @@
     </row>
     <row r="150" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>29</v>
@@ -9133,7 +9213,7 @@
         <v>23</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G150" s="6">
         <v>563</v>
@@ -9162,7 +9242,9 @@
       <c r="O150" s="6">
         <v>991</v>
       </c>
-      <c r="P150" s="3"/>
+      <c r="P150" s="6">
+        <v>1050</v>
+      </c>
       <c r="Q150" s="3"/>
       <c r="R150" s="2" t="s">
         <v>25</v>
@@ -9170,19 +9252,19 @@
     </row>
     <row r="151" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>24</v>
@@ -9219,24 +9301,24 @@
       </c>
       <c r="Q151" s="3"/>
       <c r="R151" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="152" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F152" s="3" t="s">
         <v>24</v>
@@ -9273,24 +9355,24 @@
       </c>
       <c r="Q152" s="3"/>
       <c r="R152" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="153" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F153" s="3" t="s">
         <v>24</v>
@@ -9327,24 +9409,24 @@
       </c>
       <c r="Q153" s="3"/>
       <c r="R153" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="154" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F154" s="3" t="s">
         <v>24</v>
@@ -9381,18 +9463,18 @@
       </c>
       <c r="Q154" s="3"/>
       <c r="R154" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="155" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>29</v>
@@ -9401,7 +9483,7 @@
         <v>23</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G155" s="4">
         <v>100</v>
@@ -9430,7 +9512,9 @@
       <c r="O155" s="4">
         <v>130</v>
       </c>
-      <c r="P155" s="3"/>
+      <c r="P155" s="4">
+        <v>189.5</v>
+      </c>
       <c r="Q155" s="3"/>
       <c r="R155" s="2" t="s">
         <v>25</v>
@@ -9438,13 +9522,13 @@
     </row>
     <row r="156" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>29</v>
@@ -9453,7 +9537,7 @@
         <v>23</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G156" s="4">
         <v>59.5</v>
@@ -9492,13 +9576,13 @@
     </row>
     <row r="157" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>29</v>
@@ -9507,7 +9591,7 @@
         <v>23</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G157" s="4">
         <v>88.4</v>
@@ -9541,18 +9625,18 @@
       </c>
       <c r="Q157" s="3"/>
       <c r="R157" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>29</v>
@@ -9595,18 +9679,18 @@
       </c>
       <c r="Q158" s="3"/>
       <c r="R158" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="159" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>29</v>
@@ -9654,13 +9738,13 @@
     </row>
     <row r="160" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>29</v>
@@ -9708,13 +9792,13 @@
     </row>
     <row r="161" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>29</v>
@@ -9762,13 +9846,13 @@
     </row>
     <row r="162" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>29</v>
@@ -9816,13 +9900,13 @@
     </row>
     <row r="163" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>29</v>
@@ -9867,18 +9951,18 @@
         <v>85</v>
       </c>
       <c r="R163" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>29</v>
@@ -9913,18 +9997,18 @@
         <v>74</v>
       </c>
       <c r="R164" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="165" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>29</v>
@@ -9933,7 +10017,7 @@
         <v>23</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G165" s="5">
         <v>0.98</v>
@@ -9962,7 +10046,9 @@
       <c r="O165" s="5">
         <v>0.88</v>
       </c>
-      <c r="P165" s="3"/>
+      <c r="P165" s="5">
+        <v>1.01</v>
+      </c>
       <c r="Q165" s="3"/>
       <c r="R165" s="2" t="s">
         <v>200</v>
@@ -9970,13 +10056,13 @@
     </row>
     <row r="166" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>29</v>
@@ -9985,7 +10071,7 @@
         <v>23</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G166" s="6">
         <v>830</v>
@@ -10024,13 +10110,13 @@
     </row>
     <row r="167" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>29</v>
@@ -10039,7 +10125,7 @@
         <v>23</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G167" s="5">
         <v>0.64</v>
@@ -10068,7 +10154,9 @@
       <c r="O167" s="5">
         <v>0.66</v>
       </c>
-      <c r="P167" s="3"/>
+      <c r="P167" s="5">
+        <v>0.6</v>
+      </c>
       <c r="Q167" s="3"/>
       <c r="R167" s="2" t="s">
         <v>200</v>
@@ -10076,13 +10164,13 @@
     </row>
     <row r="168" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>29</v>
@@ -10123,20 +10211,22 @@
       <c r="P168" s="6">
         <v>31</v>
       </c>
-      <c r="Q168" s="3"/>
+      <c r="Q168" s="6">
+        <v>34</v>
+      </c>
       <c r="R168" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="169" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>29</v>
@@ -10184,13 +10274,13 @@
     </row>
     <row r="170" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>29</v>
@@ -10199,7 +10289,7 @@
         <v>23</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G170" s="5">
         <v>377.75</v>
@@ -10229,22 +10319,22 @@
         <v>766.04</v>
       </c>
       <c r="P170" s="5">
-        <v>765.54</v>
+        <v>776.56</v>
       </c>
       <c r="Q170" s="3"/>
       <c r="R170" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="171" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>29</v>
@@ -10253,7 +10343,7 @@
         <v>23</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G171" s="5">
         <v>96.04</v>
@@ -10283,22 +10373,22 @@
         <v>244.93</v>
       </c>
       <c r="P171" s="5">
-        <v>221.73</v>
+        <v>223.31</v>
       </c>
       <c r="Q171" s="3"/>
       <c r="R171" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="172" spans="1:18" ht="54" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>29</v>
@@ -10341,14 +10431,14 @@
       </c>
       <c r="Q172" s="3"/>
       <c r="R172" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="173" spans="1:18" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B175" s="8"/>
     </row>

</xml_diff>

<commit_message>
okno serwisowe - excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="343">
   <si>
     <t>sdg.gov.pl/en</t>
   </si>
@@ -133,13 +133,14 @@
     <t>persons</t>
   </si>
   <si>
-    <t>Improvement of access to public services (e.g. support for families with children, child and elderly care) and health services</t>
+    <t>Improvement of access to public services (e.g. support for families with
+  children, child and elderly care) and health services</t>
   </si>
   <si>
     <t>1.3.a Percentage of children aged 1-3 covered by different kinds of institutional care</t>
   </si>
   <si>
-    <t>The Ministry of Family, Labour and Social Policy</t>
+    <t>The Ministry of Family and Social Policy</t>
   </si>
   <si>
     <t>Improvement of housing situation</t>
@@ -353,7 +354,7 @@
     <t>3.6.a Percentage of medical entities with IT solutions that enable keeping medical records in electronic form</t>
   </si>
   <si>
-    <t>Center of Information Systems for Health Care</t>
+    <t>Center of e-Health (CeZ)</t>
   </si>
   <si>
     <t>Comprehensive improvement of air quality  reaching the state of no risk to health and environment in accordance with EU legislation and, in a longer-term perspective, WHO guidelines</t>
@@ -383,36 +384,37 @@
     <t>4.2.a Percentage of foreign students studying in Polish higher education institutions in Poland</t>
   </si>
   <si>
+    <t>Creation of conditions for education development all over the country and
+  equalization of educational opportunities</t>
+  </si>
+  <si>
+    <t>4.3.a Results of PISA tests - percentage of top-performing students in reading literacy</t>
+  </si>
+  <si>
+    <t>The Organisation for Economic Co-operation and Development / the Ministry of  Education and Science</t>
+  </si>
+  <si>
+    <t>4.3.b Results of PISA tests - percentage of top-performing students in mathematics</t>
+  </si>
+  <si>
+    <t>4.3.c Results of PISA tests - percentage of the lowest-performing students in reading literacy</t>
+  </si>
+  <si>
+    <t>4.3.d Results of PISA tests - percentage of the lowest-performing students in mathematics</t>
+  </si>
+  <si>
+    <t>4.3.e Results of PISA tests - proportion of students achieving at least a minimum proficiency level in reading</t>
+  </si>
+  <si>
+    <t>4.3.f Results of PISA tests - percentage of students achieving at least a minimum proficiency level in mathematics</t>
+  </si>
+  <si>
+    <t>Organisation for Economic Co-operation and Development / the Ministry of  Education and Science</t>
+  </si>
+  <si>
     <t>Creation of conditions for education development all over the country and equalization of educational opportunities</t>
   </si>
   <si>
-    <t>4.3.a Results of PISA tests - percentage of top-performing students in reading literacy</t>
-  </si>
-  <si>
-    <t>The Organisation for Economic Co-operation and Development / the Ministry of Education</t>
-  </si>
-  <si>
-    <t>4.3.b Results of PISA tests - percentage of top-performing students in mathematics</t>
-  </si>
-  <si>
-    <t>4.3.c Results of PISA tests - percentage of the lowest-performing students in reading literacy</t>
-  </si>
-  <si>
-    <t>4.3.d Results of PISA tests - percentage of the lowest-performing students in mathematics</t>
-  </si>
-  <si>
-    <t>The Organisation for Economic Co-operation and Development / Ministry of Education</t>
-  </si>
-  <si>
-    <t>4.3.e Results of PISA tests - proportion of students achieving at least a minimum proficiency level in reading</t>
-  </si>
-  <si>
-    <t>4.3.f Results of PISA tests - percentage of students achieving at least a minimum proficiency level in mathematics</t>
-  </si>
-  <si>
-    <t>Organisation for Economic Co-operation and Development / Ministry of Education</t>
-  </si>
-  <si>
     <t>4.3.g Percentage of children aged 3-5 covered by pre-primary education</t>
   </si>
   <si>
@@ -513,6 +515,9 @@
   </si>
   <si>
     <t>5.2.a Percentage of children aged 1-3 covered by different kinds of institutional care</t>
+  </si>
+  <si>
+    <t>the Ministry of Family and Social Policy</t>
   </si>
   <si>
     <t>Ensurance of conditions for women's return to labour market after a break from employment due to childbirth and childcare</t>
@@ -582,7 +587,7 @@
     <t xml:space="preserve">minutes </t>
   </si>
   <si>
-    <t>Ministry of Energy</t>
+    <t>the Ministry of Climate and Environment</t>
   </si>
   <si>
     <t>Fulfillment of enterprises and households' energy needs</t>
@@ -1053,7 +1058,7 @@
     <t>17.2.a Official development assistance as a proportion of gross national income</t>
   </si>
   <si>
-    <t>Last update: 09-02-2021, 08:30</t>
+    <t>Last update: 16-02-2021, 11:23</t>
   </si>
 </sst>
 </file>
@@ -1597,7 +1602,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4122,7 +4127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>114</v>
       </c>
@@ -4164,7 +4169,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>114</v>
       </c>
@@ -4206,7 +4211,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>114</v>
       </c>
@@ -4248,7 +4253,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>114</v>
       </c>
@@ -4287,10 +4292,10 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>114</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>119</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>29</v>
@@ -4332,7 +4337,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>114</v>
       </c>
@@ -4340,7 +4345,7 @@
         <v>119</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>29</v>
@@ -4371,7 +4376,7 @@
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -4379,7 +4384,7 @@
         <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>129</v>
@@ -4433,7 +4438,7 @@
         <v>114</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>129</v>
@@ -4487,7 +4492,7 @@
         <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>129</v>
@@ -5571,7 +5576,7 @@
       </c>
       <c r="Q81" s="3"/>
       <c r="R81" s="2" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="27" x14ac:dyDescent="0.25">
@@ -5579,10 +5584,10 @@
         <v>148</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>29</v>
@@ -5630,13 +5635,13 @@
     </row>
     <row r="83" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>29</v>
@@ -5645,7 +5650,7 @@
         <v>23</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G83" s="4">
         <v>732401.6</v>
@@ -5677,18 +5682,18 @@
       </c>
       <c r="Q83" s="3"/>
       <c r="R83" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>29</v>
@@ -5736,13 +5741,13 @@
     </row>
     <row r="85" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>29</v>
@@ -5790,13 +5795,13 @@
     </row>
     <row r="86" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>29</v>
@@ -5844,13 +5849,13 @@
     </row>
     <row r="87" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>29</v>
@@ -5859,7 +5864,7 @@
         <v>23</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G87" s="7">
         <v>0.318</v>
@@ -5896,13 +5901,13 @@
     </row>
     <row r="88" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>29</v>
@@ -5950,13 +5955,13 @@
     </row>
     <row r="89" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>29</v>
@@ -5999,18 +6004,18 @@
       </c>
       <c r="Q89" s="3"/>
       <c r="R89" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>29</v>
@@ -6019,7 +6024,7 @@
         <v>23</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G90" s="4">
         <v>316.10000000000002</v>
@@ -6051,18 +6056,18 @@
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
       <c r="R90" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>29</v>
@@ -6108,13 +6113,13 @@
     </row>
     <row r="92" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>29</v>
@@ -6162,13 +6167,13 @@
     </row>
     <row r="93" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>29</v>
@@ -6214,13 +6219,13 @@
     </row>
     <row r="94" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>29</v>
@@ -6266,13 +6271,13 @@
     </row>
     <row r="95" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>29</v>
@@ -6281,7 +6286,7 @@
         <v>23</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G95" s="6">
         <v>39</v>
@@ -6315,18 +6320,18 @@
       </c>
       <c r="Q95" s="3"/>
       <c r="R95" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>29</v>
@@ -6335,7 +6340,7 @@
         <v>23</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -6367,18 +6372,18 @@
         <v>40</v>
       </c>
       <c r="R96" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>74</v>
@@ -6426,13 +6431,13 @@
     </row>
     <row r="98" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>74</v>
@@ -6480,13 +6485,13 @@
     </row>
     <row r="99" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>74</v>
@@ -6534,19 +6539,19 @@
     </row>
     <row r="100" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>24</v>
@@ -6588,19 +6593,19 @@
     </row>
     <row r="101" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>24</v>
@@ -6642,19 +6647,19 @@
     </row>
     <row r="102" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>24</v>
@@ -6696,19 +6701,19 @@
     </row>
     <row r="103" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>24</v>
@@ -6750,19 +6755,19 @@
     </row>
     <row r="104" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>24</v>
@@ -6804,13 +6809,13 @@
     </row>
     <row r="105" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>22</v>
@@ -6858,19 +6863,19 @@
     </row>
     <row r="106" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>24</v>
@@ -6912,13 +6917,13 @@
     </row>
     <row r="107" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>29</v>
@@ -6966,13 +6971,13 @@
     </row>
     <row r="108" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>29</v>
@@ -7020,13 +7025,13 @@
     </row>
     <row r="109" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>29</v>
@@ -7064,16 +7069,16 @@
     </row>
     <row r="110" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>23</v>
@@ -7118,16 +7123,16 @@
     </row>
     <row r="111" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>77</v>
@@ -7172,19 +7177,19 @@
     </row>
     <row r="112" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F112" s="3" t="s">
         <v>24</v>
@@ -7226,19 +7231,19 @@
     </row>
     <row r="113" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>24</v>
@@ -7280,19 +7285,19 @@
     </row>
     <row r="114" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>24</v>
@@ -7334,13 +7339,13 @@
     </row>
     <row r="115" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>29</v>
@@ -7388,13 +7393,13 @@
     </row>
     <row r="116" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>29</v>
@@ -7442,13 +7447,13 @@
     </row>
     <row r="117" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>29</v>
@@ -7496,13 +7501,13 @@
     </row>
     <row r="118" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>29</v>
@@ -7548,13 +7553,13 @@
     </row>
     <row r="119" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>29</v>
@@ -7563,7 +7568,7 @@
         <v>23</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G119" s="3"/>
       <c r="H119" s="6">
@@ -7597,18 +7602,18 @@
         <v>38</v>
       </c>
       <c r="R119" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>29</v>
@@ -7656,13 +7661,13 @@
     </row>
     <row r="121" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>29</v>
@@ -7710,13 +7715,13 @@
     </row>
     <row r="122" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>29</v>
@@ -7764,13 +7769,13 @@
     </row>
     <row r="123" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>29</v>
@@ -7816,13 +7821,13 @@
     </row>
     <row r="124" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>29</v>
@@ -7865,18 +7870,18 @@
       </c>
       <c r="Q124" s="3"/>
       <c r="R124" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>29</v>
@@ -7922,13 +7927,13 @@
     </row>
     <row r="126" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>29</v>
@@ -7963,18 +7968,18 @@
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
       <c r="R126" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>29</v>
@@ -8022,13 +8027,13 @@
     </row>
     <row r="128" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>29</v>
@@ -8076,13 +8081,13 @@
     </row>
     <row r="129" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>29</v>
@@ -8130,13 +8135,13 @@
     </row>
     <row r="130" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>29</v>
@@ -8178,13 +8183,13 @@
     </row>
     <row r="131" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>29</v>
@@ -8193,7 +8198,7 @@
         <v>23</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G131" s="4">
         <v>31.1</v>
@@ -8232,13 +8237,13 @@
     </row>
     <row r="132" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>29</v>
@@ -8286,13 +8291,13 @@
     </row>
     <row r="133" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>29</v>
@@ -8340,13 +8345,13 @@
     </row>
     <row r="134" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>29</v>
@@ -8394,13 +8399,13 @@
     </row>
     <row r="135" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>29</v>
@@ -8448,13 +8453,13 @@
     </row>
     <row r="136" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>29</v>
@@ -8497,24 +8502,24 @@
       </c>
       <c r="Q136" s="3"/>
       <c r="R136" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="137" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F137" s="3" t="s">
         <v>24</v>
@@ -8556,19 +8561,19 @@
     </row>
     <row r="138" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>24</v>
@@ -8610,19 +8615,19 @@
     </row>
     <row r="139" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F139" s="3" t="s">
         <v>24</v>
@@ -8664,19 +8669,19 @@
     </row>
     <row r="140" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F140" s="3" t="s">
         <v>24</v>
@@ -8718,13 +8723,13 @@
     </row>
     <row r="141" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>29</v>
@@ -8772,13 +8777,13 @@
     </row>
     <row r="142" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>29</v>
@@ -8787,7 +8792,7 @@
         <v>23</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G142" s="4">
         <v>20.8</v>
@@ -8826,13 +8831,13 @@
     </row>
     <row r="143" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>29</v>
@@ -8841,7 +8846,7 @@
         <v>23</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G143" s="5">
         <v>0.56000000000000005</v>
@@ -8880,13 +8885,13 @@
     </row>
     <row r="144" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>29</v>
@@ -8895,7 +8900,7 @@
         <v>23</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G144" s="5">
         <v>16.95</v>
@@ -8934,13 +8939,13 @@
     </row>
     <row r="145" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>29</v>
@@ -8988,13 +8993,13 @@
     </row>
     <row r="146" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>29</v>
@@ -9042,13 +9047,13 @@
     </row>
     <row r="147" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>29</v>
@@ -9057,7 +9062,7 @@
         <v>23</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G147" s="4">
         <v>100</v>
@@ -9089,18 +9094,18 @@
       <c r="P147" s="3"/>
       <c r="Q147" s="3"/>
       <c r="R147" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="148" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>29</v>
@@ -9109,7 +9114,7 @@
         <v>23</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G148" s="4">
         <v>100</v>
@@ -9141,18 +9146,18 @@
       <c r="P148" s="3"/>
       <c r="Q148" s="3"/>
       <c r="R148" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="149" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>29</v>
@@ -9200,13 +9205,13 @@
     </row>
     <row r="150" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>29</v>
@@ -9215,7 +9220,7 @@
         <v>23</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G150" s="6">
         <v>563</v>
@@ -9254,19 +9259,19 @@
     </row>
     <row r="151" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>24</v>
@@ -9303,24 +9308,24 @@
       </c>
       <c r="Q151" s="3"/>
       <c r="R151" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="152" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F152" s="3" t="s">
         <v>24</v>
@@ -9357,24 +9362,24 @@
       </c>
       <c r="Q152" s="3"/>
       <c r="R152" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="153" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F153" s="3" t="s">
         <v>24</v>
@@ -9411,24 +9416,24 @@
       </c>
       <c r="Q153" s="3"/>
       <c r="R153" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="154" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F154" s="3" t="s">
         <v>24</v>
@@ -9465,18 +9470,18 @@
       </c>
       <c r="Q154" s="3"/>
       <c r="R154" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="155" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>29</v>
@@ -9485,7 +9490,7 @@
         <v>23</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G155" s="4">
         <v>100</v>
@@ -9524,13 +9529,13 @@
     </row>
     <row r="156" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>29</v>
@@ -9539,7 +9544,7 @@
         <v>23</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G156" s="4">
         <v>59.5</v>
@@ -9578,13 +9583,13 @@
     </row>
     <row r="157" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>29</v>
@@ -9593,7 +9598,7 @@
         <v>23</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G157" s="4">
         <v>88.4</v>
@@ -9627,18 +9632,18 @@
       </c>
       <c r="Q157" s="3"/>
       <c r="R157" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="158" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>29</v>
@@ -9681,18 +9686,18 @@
       </c>
       <c r="Q158" s="3"/>
       <c r="R158" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="159" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>29</v>
@@ -9740,13 +9745,13 @@
     </row>
     <row r="160" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>29</v>
@@ -9794,13 +9799,13 @@
     </row>
     <row r="161" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>29</v>
@@ -9848,13 +9853,13 @@
     </row>
     <row r="162" spans="1:18" ht="36" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>29</v>
@@ -9902,13 +9907,13 @@
     </row>
     <row r="163" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>29</v>
@@ -9953,18 +9958,18 @@
         <v>85</v>
       </c>
       <c r="R163" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="164" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>29</v>
@@ -9999,18 +10004,18 @@
         <v>74</v>
       </c>
       <c r="R164" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="165" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>29</v>
@@ -10019,7 +10024,7 @@
         <v>23</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G165" s="5">
         <v>0.98</v>
@@ -10053,18 +10058,18 @@
       </c>
       <c r="Q165" s="3"/>
       <c r="R165" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="166" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>29</v>
@@ -10073,7 +10078,7 @@
         <v>23</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G166" s="6">
         <v>830</v>
@@ -10107,18 +10112,18 @@
       </c>
       <c r="Q166" s="3"/>
       <c r="R166" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="167" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>29</v>
@@ -10127,7 +10132,7 @@
         <v>23</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G167" s="5">
         <v>0.64</v>
@@ -10161,18 +10166,18 @@
       </c>
       <c r="Q167" s="3"/>
       <c r="R167" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="168" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>29</v>
@@ -10222,13 +10227,13 @@
     </row>
     <row r="169" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>29</v>
@@ -10276,13 +10281,13 @@
     </row>
     <row r="170" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>29</v>
@@ -10291,7 +10296,7 @@
         <v>23</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G170" s="5">
         <v>377.75</v>
@@ -10325,18 +10330,18 @@
       </c>
       <c r="Q170" s="3"/>
       <c r="R170" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="171" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>29</v>
@@ -10345,7 +10350,7 @@
         <v>23</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G171" s="5">
         <v>96.04</v>
@@ -10379,18 +10384,18 @@
       </c>
       <c r="Q171" s="3"/>
       <c r="R171" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="172" spans="1:18" ht="54" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>29</v>
@@ -10433,14 +10438,14 @@
       </c>
       <c r="Q172" s="3"/>
       <c r="R172" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="173" spans="1:18" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B175" s="8"/>
     </row>
@@ -10455,7 +10460,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aktualizacja plików Excel (poprawki)
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -1282,7 +1282,7 @@
     <t>17.2.a Official development assistance as a proportion of gross national income</t>
   </si>
   <si>
-    <t>Last update: 04-04-2023, 13:52</t>
+    <t>Last update: 06-04-2023, 11:56</t>
   </si>
 </sst>
 </file>
@@ -17021,41 +17021,37 @@
       <c r="F289" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G289" s="4">
-        <v>41.6</v>
-      </c>
-      <c r="H289" s="4">
-        <v>44.7</v>
-      </c>
+      <c r="G289" s="3"/>
+      <c r="H289" s="3"/>
       <c r="I289" s="4">
-        <v>46.5</v>
+        <v>29.8</v>
       </c>
       <c r="J289" s="4">
-        <v>48.2</v>
+        <v>31.1</v>
       </c>
       <c r="K289" s="4">
-        <v>49.6</v>
+        <v>30.3</v>
       </c>
       <c r="L289" s="4">
-        <v>49.8</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="M289" s="4">
-        <v>50.6</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="N289" s="4">
-        <v>51.2</v>
+        <v>35.6</v>
       </c>
       <c r="O289" s="4">
-        <v>52.4</v>
+        <v>37.5</v>
       </c>
       <c r="P289" s="4">
-        <v>53.4</v>
+        <v>35.9</v>
       </c>
       <c r="Q289" s="4">
-        <v>53.9</v>
+        <v>36.6</v>
       </c>
       <c r="R289" s="4">
-        <v>54.8</v>
+        <v>36.1</v>
       </c>
       <c r="S289" s="3"/>
       <c r="T289" s="2" t="s">
@@ -17083,36 +17079,18 @@
       </c>
       <c r="G290" s="3"/>
       <c r="H290" s="3"/>
-      <c r="I290" s="4">
-        <v>29.8</v>
-      </c>
-      <c r="J290" s="4">
-        <v>31.1</v>
-      </c>
-      <c r="K290" s="4">
-        <v>30.3</v>
-      </c>
-      <c r="L290" s="4">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="M290" s="4">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="N290" s="4">
-        <v>35.6</v>
-      </c>
-      <c r="O290" s="4">
-        <v>37.5</v>
-      </c>
-      <c r="P290" s="4">
-        <v>35.9</v>
-      </c>
-      <c r="Q290" s="4">
-        <v>36.6</v>
-      </c>
-      <c r="R290" s="4">
-        <v>36.1</v>
-      </c>
+      <c r="I290" s="3"/>
+      <c r="J290" s="3"/>
+      <c r="K290" s="3"/>
+      <c r="L290" s="3"/>
+      <c r="M290" s="3"/>
+      <c r="N290" s="3"/>
+      <c r="O290" s="3"/>
+      <c r="P290" s="3"/>
+      <c r="Q290" s="5">
+        <v>83.49</v>
+      </c>
+      <c r="R290" s="3"/>
       <c r="S290" s="3"/>
       <c r="T290" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Okno serwisowe 25.07.2023 - aktualizacja excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niewiadomskaew\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="18060" windowHeight="7050"/>
   </bookViews>
@@ -1244,20 +1249,20 @@
     <t>17.6.a Conferences and trainings conducted by National Revenue Administration experts in countries covered by assistance</t>
   </si>
   <si>
-    <t>Last update: 04-07-2023, 11:49</t>
+    <t>Last update: 25-07-2023, 10:38</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-10809]0.0;\-0.0;0.0"/>
     <numFmt numFmtId="165" formatCode="[$-10809]0.00;\-0.00;0.00"/>
     <numFmt numFmtId="166" formatCode="[$-10809]0;\-0;0"/>
     <numFmt numFmtId="167" formatCode="[$-10809]0.000;\-0.000;0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1449,6 +1454,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1469,7 +1482,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1532,7 +1545,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1564,9 +1577,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1598,6 +1612,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -1773,15 +1788,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T300"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
@@ -1794,17 +1809,17 @@
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" customHeight="1">
+    <row r="1" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:20" ht="25.5">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1866,7 +1881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="29.25">
+    <row r="4" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1922,7 +1937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="29.25">
+    <row r="5" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1978,7 +1993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="29.25">
+    <row r="6" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2038,7 +2053,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="29.25">
+    <row r="7" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2096,7 +2111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="29.25">
+    <row r="8" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2154,7 +2169,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -2209,12 +2224,14 @@
       <c r="R9" s="4">
         <v>405.2</v>
       </c>
-      <c r="S9" s="3"/>
+      <c r="S9" s="4">
+        <v>412.4</v>
+      </c>
       <c r="T9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2269,12 +2286,14 @@
       <c r="R10" s="4">
         <v>460.3</v>
       </c>
-      <c r="S10" s="3"/>
+      <c r="S10" s="4">
+        <v>469.6</v>
+      </c>
       <c r="T10" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2329,12 +2348,14 @@
       <c r="R11" s="4">
         <v>323.7</v>
       </c>
-      <c r="S11" s="3"/>
+      <c r="S11" s="4">
+        <v>328.2</v>
+      </c>
       <c r="T11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="39">
+    <row r="12" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
@@ -2394,7 +2415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="29.25">
+    <row r="13" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -2454,7 +2475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="29.25">
+    <row r="14" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2512,7 +2533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="29.25">
+    <row r="15" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -2570,7 +2591,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="29.25">
+    <row r="16" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -2628,7 +2649,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="39">
+    <row r="17" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -2688,7 +2709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="29.25">
+    <row r="18" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
@@ -2748,7 +2769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="29.25">
+    <row r="19" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -2808,7 +2829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="19.5">
+    <row r="20" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -2850,7 +2871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="19.5">
+    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -2892,7 +2913,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="19.5">
+    <row r="22" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
@@ -2934,7 +2955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="19.5">
+    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -2976,7 +2997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="19.5">
+    <row r="24" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -3036,7 +3057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="19.5">
+    <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -3096,7 +3117,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="19.5">
+    <row r="26" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -3156,7 +3177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="19.5">
+    <row r="27" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>63</v>
       </c>
@@ -3216,7 +3237,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="19.5">
+    <row r="28" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -3276,7 +3297,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="19.5">
+    <row r="29" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>63</v>
       </c>
@@ -3336,7 +3357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="19.5">
+    <row r="30" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>63</v>
       </c>
@@ -3396,7 +3417,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="19.5">
+    <row r="31" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -3456,7 +3477,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="19.5">
+    <row r="32" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -3516,7 +3537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="19.5">
+    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -3576,7 +3597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="19.5">
+    <row r="34" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>63</v>
       </c>
@@ -3636,7 +3657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="19.5">
+    <row r="35" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>63</v>
       </c>
@@ -3696,7 +3717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="19.5">
+    <row r="36" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
@@ -3756,7 +3777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="19.5">
+    <row r="37" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
@@ -3816,7 +3837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="19.5">
+    <row r="38" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
@@ -3876,7 +3897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="19.5">
+    <row r="39" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>63</v>
       </c>
@@ -3936,7 +3957,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="19.5">
+    <row r="40" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>63</v>
       </c>
@@ -3996,7 +4017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="19.5">
+    <row r="41" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>63</v>
       </c>
@@ -4056,7 +4077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="19.5">
+    <row r="42" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>
@@ -4116,7 +4137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="19.5">
+    <row r="43" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>63</v>
       </c>
@@ -4176,7 +4197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="19.5">
+    <row r="44" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
@@ -4236,7 +4257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="19.5">
+    <row r="45" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>63</v>
       </c>
@@ -4296,7 +4317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="19.5">
+    <row r="46" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>63</v>
       </c>
@@ -4338,7 +4359,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="19.5">
+    <row r="47" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>63</v>
       </c>
@@ -4380,7 +4401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="19.5">
+    <row r="48" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -4422,7 +4443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="19.5">
+    <row r="49" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>63</v>
       </c>
@@ -4464,7 +4485,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="19.5">
+    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>63</v>
       </c>
@@ -4506,7 +4527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="19.5">
+    <row r="51" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>63</v>
       </c>
@@ -4548,7 +4569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="19.5">
+    <row r="52" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>63</v>
       </c>
@@ -4590,7 +4611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="19.5">
+    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
@@ -4632,7 +4653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="19.5">
+    <row r="54" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
@@ -4674,7 +4695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="19.5">
+    <row r="55" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>63</v>
       </c>
@@ -4716,7 +4737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="19.5">
+    <row r="56" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -4758,7 +4779,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="19.5">
+    <row r="57" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>63</v>
       </c>
@@ -4800,7 +4821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="19.5">
+    <row r="58" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
@@ -4840,7 +4861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="19.5">
+    <row r="59" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
@@ -4880,7 +4901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="19.5">
+    <row r="60" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>63</v>
       </c>
@@ -4920,7 +4941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="19.5">
+    <row r="61" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
@@ -4982,7 +5003,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="29.25">
+    <row r="62" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
@@ -5042,7 +5063,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="29.25">
+    <row r="63" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -5094,7 +5115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="29.25">
+    <row r="64" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
@@ -5146,7 +5167,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="29.25">
+    <row r="65" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -5198,7 +5219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="29.25">
+    <row r="66" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>63</v>
       </c>
@@ -5242,7 +5263,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="48.75">
+    <row r="67" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>63</v>
       </c>
@@ -5302,7 +5323,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="39">
+    <row r="68" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>100</v>
       </c>
@@ -5357,12 +5378,14 @@
       <c r="R68" s="4">
         <v>28.8</v>
       </c>
-      <c r="S68" s="3"/>
+      <c r="S68" s="4">
+        <v>36.1</v>
+      </c>
       <c r="T68" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="39">
+    <row r="69" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>100</v>
       </c>
@@ -5406,7 +5429,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="48.75">
+    <row r="70" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>100</v>
       </c>
@@ -5450,7 +5473,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="48.75">
+    <row r="71" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>100</v>
       </c>
@@ -5494,7 +5517,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="48.75">
+    <row r="72" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>100</v>
       </c>
@@ -5538,7 +5561,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="48.75">
+    <row r="73" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>100</v>
       </c>
@@ -5582,7 +5605,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="48.75">
+    <row r="74" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>100</v>
       </c>
@@ -5626,7 +5649,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="48.75">
+    <row r="75" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>100</v>
       </c>
@@ -5670,7 +5693,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="29.25">
+    <row r="76" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>100</v>
       </c>
@@ -5730,7 +5753,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="29.25">
+    <row r="77" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
@@ -5790,7 +5813,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="29.25">
+    <row r="78" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>100</v>
       </c>
@@ -5850,7 +5873,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="39">
+    <row r="79" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>100</v>
       </c>
@@ -5912,7 +5935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="39">
+    <row r="80" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>100</v>
       </c>
@@ -5974,7 +5997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="39">
+    <row r="81" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>100</v>
       </c>
@@ -6036,7 +6059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="39">
+    <row r="82" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>100</v>
       </c>
@@ -6091,12 +6114,14 @@
       <c r="R82" s="4">
         <v>5.4</v>
       </c>
-      <c r="S82" s="3"/>
+      <c r="S82" s="4">
+        <v>7.6</v>
+      </c>
       <c r="T82" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="39">
+    <row r="83" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
@@ -6151,12 +6176,14 @@
       <c r="R83" s="4">
         <v>8.1</v>
       </c>
-      <c r="S83" s="3"/>
+      <c r="S83" s="4">
+        <v>11.3</v>
+      </c>
       <c r="T83" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="39">
+    <row r="84" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>100</v>
       </c>
@@ -6211,12 +6238,14 @@
       <c r="R84" s="4">
         <v>6.9</v>
       </c>
-      <c r="S84" s="3"/>
+      <c r="S84" s="4">
+        <v>9.4</v>
+      </c>
       <c r="T84" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="39">
+    <row r="85" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>100</v>
       </c>
@@ -6271,12 +6300,14 @@
       <c r="R85" s="4">
         <v>4.5</v>
       </c>
-      <c r="S85" s="3"/>
+      <c r="S85" s="4">
+        <v>6.4</v>
+      </c>
       <c r="T85" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="39">
+    <row r="86" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>100</v>
       </c>
@@ -6331,12 +6362,14 @@
       <c r="R86" s="4">
         <v>6.7</v>
       </c>
-      <c r="S86" s="3"/>
+      <c r="S86" s="4">
+        <v>9</v>
+      </c>
       <c r="T86" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="39">
+    <row r="87" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>100</v>
       </c>
@@ -6391,12 +6424,14 @@
       <c r="R87" s="4">
         <v>4.7</v>
       </c>
-      <c r="S87" s="3"/>
+      <c r="S87" s="4">
+        <v>6.6</v>
+      </c>
       <c r="T87" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="39">
+    <row r="88" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
@@ -6451,12 +6486,14 @@
       <c r="R88" s="4">
         <v>1.8</v>
       </c>
-      <c r="S88" s="3"/>
+      <c r="S88" s="4">
+        <v>2.9</v>
+      </c>
       <c r="T88" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="39">
+    <row r="89" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>100</v>
       </c>
@@ -6511,12 +6548,14 @@
       <c r="R89" s="4">
         <v>2</v>
       </c>
-      <c r="S89" s="3"/>
+      <c r="S89" s="4">
+        <v>3.3</v>
+      </c>
       <c r="T89" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="29.25">
+    <row r="90" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>100</v>
       </c>
@@ -6556,7 +6595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="29.25">
+    <row r="91" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>100</v>
       </c>
@@ -6594,7 +6633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="29.25">
+    <row r="92" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>100</v>
       </c>
@@ -6632,7 +6671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="29.25">
+    <row r="93" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>100</v>
       </c>
@@ -6670,7 +6709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="29.25">
+    <row r="94" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
@@ -6708,7 +6747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="29.25">
+    <row r="95" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>100</v>
       </c>
@@ -6746,7 +6785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="29.25">
+    <row r="96" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
@@ -6784,7 +6823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="19.5">
+    <row r="97" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -6822,7 +6861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="19.5">
+    <row r="98" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
@@ -6860,7 +6899,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="19.5">
+    <row r="99" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>100</v>
       </c>
@@ -6898,7 +6937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="19.5">
+    <row r="100" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
@@ -6936,7 +6975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="19.5">
+    <row r="101" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -6974,7 +7013,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="19.5">
+    <row r="102" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -7012,7 +7051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="19.5">
+    <row r="103" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>100</v>
       </c>
@@ -7050,7 +7089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="19.5">
+    <row r="104" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>100</v>
       </c>
@@ -7088,7 +7127,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="19.5">
+    <row r="105" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>100</v>
       </c>
@@ -7126,7 +7165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="19.5">
+    <row r="106" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>100</v>
       </c>
@@ -7164,7 +7203,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="19.5">
+    <row r="107" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>100</v>
       </c>
@@ -7202,7 +7241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="19.5">
+    <row r="108" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>100</v>
       </c>
@@ -7240,7 +7279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="19.5">
+    <row r="109" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>100</v>
       </c>
@@ -7278,7 +7317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="19.5">
+    <row r="110" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>100</v>
       </c>
@@ -7316,7 +7355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="19.5">
+    <row r="111" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>100</v>
       </c>
@@ -7354,7 +7393,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="19.5">
+    <row r="112" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>100</v>
       </c>
@@ -7392,7 +7431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="19.5">
+    <row r="113" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>100</v>
       </c>
@@ -7430,7 +7469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="19.5">
+    <row r="114" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>100</v>
       </c>
@@ -7468,7 +7507,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="19.5">
+    <row r="115" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>149</v>
       </c>
@@ -7528,7 +7567,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="19.5">
+    <row r="116" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>149</v>
       </c>
@@ -7590,7 +7629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="19.5">
+    <row r="117" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>149</v>
       </c>
@@ -7652,7 +7691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="19.5">
+    <row r="118" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>149</v>
       </c>
@@ -7714,7 +7753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="19.5">
+    <row r="119" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>149</v>
       </c>
@@ -7762,7 +7801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="39">
+    <row r="120" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>149</v>
       </c>
@@ -7810,7 +7849,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="19.5">
+    <row r="121" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>149</v>
       </c>
@@ -7858,7 +7897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="39">
+    <row r="122" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>149</v>
       </c>
@@ -7906,7 +7945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="39">
+    <row r="123" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>149</v>
       </c>
@@ -7954,7 +7993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="39">
+    <row r="124" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>149</v>
       </c>
@@ -8002,7 +8041,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="39">
+    <row r="125" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>149</v>
       </c>
@@ -8050,7 +8089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="19.5">
+    <row r="126" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>149</v>
       </c>
@@ -8110,7 +8149,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="19.5">
+    <row r="127" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>149</v>
       </c>
@@ -8168,7 +8207,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="19.5">
+    <row r="128" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>149</v>
       </c>
@@ -8226,7 +8265,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="29.25">
+    <row r="129" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>149</v>
       </c>
@@ -8281,12 +8320,14 @@
       <c r="R129" s="4">
         <v>69.2</v>
       </c>
-      <c r="S129" s="3"/>
+      <c r="S129" s="4">
+        <v>71.900000000000006</v>
+      </c>
       <c r="T129" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="29.25">
+    <row r="130" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>149</v>
       </c>
@@ -8341,12 +8382,14 @@
       <c r="R130" s="4">
         <v>75.7</v>
       </c>
-      <c r="S130" s="3"/>
+      <c r="S130" s="4">
+        <v>77.3</v>
+      </c>
       <c r="T130" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="29.25">
+    <row r="131" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>149</v>
       </c>
@@ -8401,12 +8444,14 @@
       <c r="R131" s="4">
         <v>60.6</v>
       </c>
-      <c r="S131" s="3"/>
+      <c r="S131" s="4">
+        <v>65.099999999999994</v>
+      </c>
       <c r="T131" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="29.25">
+    <row r="132" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>167</v>
       </c>
@@ -8459,12 +8504,14 @@
       <c r="R132" s="4">
         <v>855928.1</v>
       </c>
-      <c r="S132" s="3"/>
+      <c r="S132" s="4">
+        <v>859996.9</v>
+      </c>
       <c r="T132" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="29.25">
+    <row r="133" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>167</v>
       </c>
@@ -8524,7 +8571,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="39">
+    <row r="134" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>167</v>
       </c>
@@ -8584,7 +8631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="39">
+    <row r="135" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>167</v>
       </c>
@@ -8644,7 +8691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="39">
+    <row r="136" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>167</v>
       </c>
@@ -8704,7 +8751,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="39">
+    <row r="137" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>167</v>
       </c>
@@ -8764,7 +8811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="29.25">
+    <row r="138" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>176</v>
       </c>
@@ -8822,7 +8869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="29.25">
+    <row r="139" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>176</v>
       </c>
@@ -8882,7 +8929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="29.25">
+    <row r="140" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>176</v>
       </c>
@@ -8942,7 +8989,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="19.5">
+    <row r="141" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>176</v>
       </c>
@@ -9002,7 +9049,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="39">
+    <row r="142" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>188</v>
       </c>
@@ -9062,7 +9109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="39">
+    <row r="143" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>188</v>
       </c>
@@ -9122,7 +9169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="39">
+    <row r="144" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>188</v>
       </c>
@@ -9178,7 +9225,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="29.25">
+    <row r="145" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>188</v>
       </c>
@@ -9230,7 +9277,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="29.25">
+    <row r="146" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>188</v>
       </c>
@@ -9285,12 +9332,14 @@
       <c r="R146" s="4">
         <v>55.8</v>
       </c>
-      <c r="S146" s="3"/>
+      <c r="S146" s="4">
+        <v>56.3</v>
+      </c>
       <c r="T146" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="29.25">
+    <row r="147" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>188</v>
       </c>
@@ -9345,12 +9394,14 @@
       <c r="R147" s="4">
         <v>63.8</v>
       </c>
-      <c r="S147" s="3"/>
+      <c r="S147" s="4">
+        <v>64</v>
+      </c>
       <c r="T147" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="29.25">
+    <row r="148" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>188</v>
       </c>
@@ -9405,12 +9456,14 @@
       <c r="R148" s="4">
         <v>48.5</v>
       </c>
-      <c r="S148" s="3"/>
+      <c r="S148" s="4">
+        <v>49.3</v>
+      </c>
       <c r="T148" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="29.25">
+    <row r="149" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>188</v>
       </c>
@@ -9465,12 +9518,14 @@
       <c r="R149" s="4">
         <v>27.3</v>
       </c>
-      <c r="S149" s="3"/>
+      <c r="S149" s="4">
+        <v>27.8</v>
+      </c>
       <c r="T149" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="29.25">
+    <row r="150" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>188</v>
       </c>
@@ -9525,12 +9580,14 @@
       <c r="R150" s="4">
         <v>70.3</v>
       </c>
-      <c r="S150" s="3"/>
+      <c r="S150" s="4">
+        <v>71.3</v>
+      </c>
       <c r="T150" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="29.25">
+    <row r="151" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>188</v>
       </c>
@@ -9585,12 +9642,14 @@
       <c r="R151" s="4">
         <v>76.599999999999994</v>
       </c>
-      <c r="S151" s="3"/>
+      <c r="S151" s="4">
+        <v>77.8</v>
+      </c>
       <c r="T151" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="29.25">
+    <row r="152" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>188</v>
       </c>
@@ -9645,12 +9704,14 @@
       <c r="R152" s="4">
         <v>49.3</v>
       </c>
-      <c r="S152" s="3"/>
+      <c r="S152" s="4">
+        <v>51</v>
+      </c>
       <c r="T152" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="29.25">
+    <row r="153" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>188</v>
       </c>
@@ -9705,12 +9766,14 @@
       <c r="R153" s="4">
         <v>75.400000000000006</v>
       </c>
-      <c r="S153" s="3"/>
+      <c r="S153" s="4">
+        <v>76.7</v>
+      </c>
       <c r="T153" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="29.25">
+    <row r="154" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>188</v>
       </c>
@@ -9765,12 +9828,14 @@
       <c r="R154" s="4">
         <v>34.700000000000003</v>
       </c>
-      <c r="S154" s="3"/>
+      <c r="S154" s="4">
+        <v>35.1</v>
+      </c>
       <c r="T154" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="29.25">
+    <row r="155" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>188</v>
       </c>
@@ -9825,12 +9890,14 @@
       <c r="R155" s="4">
         <v>54.7</v>
       </c>
-      <c r="S155" s="3"/>
+      <c r="S155" s="4">
+        <v>56.4</v>
+      </c>
       <c r="T155" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="29.25">
+    <row r="156" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>188</v>
       </c>
@@ -9885,12 +9952,14 @@
       <c r="R156" s="4">
         <v>11.5</v>
       </c>
-      <c r="S156" s="3"/>
+      <c r="S156" s="4">
+        <v>12.3</v>
+      </c>
       <c r="T156" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="29.25">
+    <row r="157" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>188</v>
       </c>
@@ -9945,12 +10014,14 @@
       <c r="R157" s="4">
         <v>56</v>
       </c>
-      <c r="S157" s="3"/>
+      <c r="S157" s="4">
+        <v>56.3</v>
+      </c>
       <c r="T157" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="29.25">
+    <row r="158" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>188</v>
       </c>
@@ -10005,12 +10076,14 @@
       <c r="R158" s="4">
         <v>55.5</v>
       </c>
-      <c r="S158" s="3"/>
+      <c r="S158" s="4">
+        <v>56.3</v>
+      </c>
       <c r="T158" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="29.25">
+    <row r="159" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>188</v>
       </c>
@@ -10065,12 +10138,14 @@
       <c r="R159" s="4">
         <v>79.7</v>
       </c>
-      <c r="S159" s="3"/>
+      <c r="S159" s="4">
+        <v>80.3</v>
+      </c>
       <c r="T159" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="29.25">
+    <row r="160" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>188</v>
       </c>
@@ -10125,12 +10200,14 @@
       <c r="R160" s="4">
         <v>59.8</v>
       </c>
-      <c r="S160" s="3"/>
+      <c r="S160" s="4">
+        <v>59.9</v>
+      </c>
       <c r="T160" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="29.25">
+    <row r="161" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>188</v>
       </c>
@@ -10185,12 +10262,14 @@
       <c r="R161" s="4">
         <v>51</v>
       </c>
-      <c r="S161" s="3"/>
+      <c r="S161" s="4">
+        <v>52.5</v>
+      </c>
       <c r="T161" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="29.25">
+    <row r="162" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>188</v>
       </c>
@@ -10245,12 +10324,14 @@
       <c r="R162" s="4">
         <v>53.2</v>
       </c>
-      <c r="S162" s="3"/>
+      <c r="S162" s="4">
+        <v>53.2</v>
+      </c>
       <c r="T162" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="48.75">
+    <row r="163" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>188</v>
       </c>
@@ -10305,12 +10386,14 @@
       <c r="R163" s="4">
         <v>16.5</v>
       </c>
-      <c r="S163" s="3"/>
+      <c r="S163" s="4">
+        <v>16.3</v>
+      </c>
       <c r="T163" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="29.25">
+    <row r="164" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>188</v>
       </c>
@@ -10370,7 +10453,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="29.25">
+    <row r="165" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>188</v>
       </c>
@@ -10430,7 +10513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="29.25">
+    <row r="166" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>188</v>
       </c>
@@ -10490,7 +10573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="29.25">
+    <row r="167" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>188</v>
       </c>
@@ -10545,12 +10628,14 @@
       <c r="R167" s="4">
         <v>57.8</v>
       </c>
-      <c r="S167" s="3"/>
+      <c r="S167" s="4">
+        <v>58</v>
+      </c>
       <c r="T167" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="29.25">
+    <row r="168" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>188</v>
       </c>
@@ -10605,12 +10690,14 @@
       <c r="R168" s="4">
         <v>50.2</v>
       </c>
-      <c r="S168" s="3"/>
+      <c r="S168" s="4">
+        <v>50.8</v>
+      </c>
       <c r="T168" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="29.25">
+    <row r="169" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>188</v>
       </c>
@@ -10665,12 +10752,14 @@
       <c r="R169" s="4">
         <v>66</v>
       </c>
-      <c r="S169" s="3"/>
+      <c r="S169" s="4">
+        <v>65.8</v>
+      </c>
       <c r="T169" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="29.25">
+    <row r="170" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>188</v>
       </c>
@@ -10725,12 +10814,14 @@
       <c r="R170" s="4">
         <v>58</v>
       </c>
-      <c r="S170" s="3"/>
+      <c r="S170" s="4">
+        <v>57.9</v>
+      </c>
       <c r="T170" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="29.25">
+    <row r="171" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>188</v>
       </c>
@@ -10785,12 +10876,14 @@
       <c r="R171" s="4">
         <v>57.4</v>
       </c>
-      <c r="S171" s="3"/>
+      <c r="S171" s="4">
+        <v>58.1</v>
+      </c>
       <c r="T171" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="29.25">
+    <row r="172" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>188</v>
       </c>
@@ -10845,12 +10938,14 @@
       <c r="R172" s="4">
         <v>31</v>
       </c>
-      <c r="S172" s="3"/>
+      <c r="S172" s="4">
+        <v>31.1</v>
+      </c>
       <c r="T172" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="29.25">
+    <row r="173" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>188</v>
       </c>
@@ -10905,12 +11000,14 @@
       <c r="R173" s="4">
         <v>79.400000000000006</v>
       </c>
-      <c r="S173" s="3"/>
+      <c r="S173" s="4">
+        <v>80.2</v>
+      </c>
       <c r="T173" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="29.25">
+    <row r="174" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>188</v>
       </c>
@@ -10965,12 +11062,14 @@
       <c r="R174" s="4">
         <v>35.6</v>
       </c>
-      <c r="S174" s="3"/>
+      <c r="S174" s="4">
+        <v>35.799999999999997</v>
+      </c>
       <c r="T174" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="29.25">
+    <row r="175" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>188</v>
       </c>
@@ -11025,12 +11124,14 @@
       <c r="R175" s="4">
         <v>19.5</v>
       </c>
-      <c r="S175" s="3"/>
+      <c r="S175" s="4">
+        <v>20.100000000000001</v>
+      </c>
       <c r="T175" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="29.25">
+    <row r="176" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>188</v>
       </c>
@@ -11085,12 +11186,14 @@
       <c r="R176" s="4">
         <v>18.100000000000001</v>
       </c>
-      <c r="S176" s="3"/>
+      <c r="S176" s="4">
+        <v>22.1</v>
+      </c>
       <c r="T176" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="29.25">
+    <row r="177" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>188</v>
       </c>
@@ -11145,12 +11248,14 @@
       <c r="R177" s="4">
         <v>19.3</v>
       </c>
-      <c r="S177" s="3"/>
+      <c r="S177" s="4">
+        <v>21.3</v>
+      </c>
       <c r="T177" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="29.25">
+    <row r="178" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>188</v>
       </c>
@@ -11205,12 +11310,14 @@
       <c r="R178" s="4">
         <v>17.5</v>
       </c>
-      <c r="S178" s="3"/>
+      <c r="S178" s="4">
+        <v>22.8</v>
+      </c>
       <c r="T178" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="29.25">
+    <row r="179" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>188</v>
       </c>
@@ -11265,12 +11372,14 @@
       <c r="R179" s="4">
         <v>17.5</v>
       </c>
-      <c r="S179" s="3"/>
+      <c r="S179" s="4">
+        <v>21</v>
+      </c>
       <c r="T179" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="29.25">
+    <row r="180" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>188</v>
       </c>
@@ -11325,12 +11434,14 @@
       <c r="R180" s="4">
         <v>19</v>
       </c>
-      <c r="S180" s="3"/>
+      <c r="S180" s="4">
+        <v>23.6</v>
+      </c>
       <c r="T180" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="29.25">
+    <row r="181" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>188</v>
       </c>
@@ -11385,12 +11496,14 @@
       <c r="R181" s="4">
         <v>11.2</v>
       </c>
-      <c r="S181" s="3"/>
+      <c r="S181" s="4">
+        <v>8</v>
+      </c>
       <c r="T181" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="29.25">
+    <row r="182" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>188</v>
       </c>
@@ -11445,12 +11558,14 @@
       <c r="R182" s="4">
         <v>11.9</v>
       </c>
-      <c r="S182" s="3"/>
+      <c r="S182" s="4">
+        <v>8.6</v>
+      </c>
       <c r="T182" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="29.25">
+    <row r="183" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>188</v>
       </c>
@@ -11505,12 +11620,14 @@
       <c r="R183" s="4">
         <v>10.5</v>
       </c>
-      <c r="S183" s="3"/>
+      <c r="S183" s="4">
+        <v>7.5</v>
+      </c>
       <c r="T183" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="29.25">
+    <row r="184" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>188</v>
       </c>
@@ -11563,12 +11680,14 @@
       <c r="R184" s="6">
         <v>3404</v>
       </c>
-      <c r="S184" s="3"/>
+      <c r="S184" s="6">
+        <v>1939</v>
+      </c>
       <c r="T184" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="29.25">
+    <row r="185" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>188</v>
       </c>
@@ -11621,12 +11740,14 @@
       <c r="R185" s="6">
         <v>1043</v>
       </c>
-      <c r="S185" s="3"/>
+      <c r="S185" s="6">
+        <v>2234</v>
+      </c>
       <c r="T185" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="29.25">
+    <row r="186" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>188</v>
       </c>
@@ -11679,12 +11800,14 @@
       <c r="R186" s="6">
         <v>2361</v>
       </c>
-      <c r="S186" s="3"/>
+      <c r="S186" s="6">
+        <v>-295</v>
+      </c>
       <c r="T186" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="29.25">
+    <row r="187" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>223</v>
       </c>
@@ -11744,7 +11867,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="29.25">
+    <row r="188" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>223</v>
       </c>
@@ -11804,7 +11927,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="29.25">
+    <row r="189" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>223</v>
       </c>
@@ -11864,7 +11987,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="39">
+    <row r="190" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>223</v>
       </c>
@@ -11918,7 +12041,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="29.25">
+    <row r="191" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>223</v>
       </c>
@@ -11978,7 +12101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="19.5">
+    <row r="192" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>237</v>
       </c>
@@ -12036,7 +12159,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="19.5">
+    <row r="193" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>237</v>
       </c>
@@ -12096,7 +12219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="19.5">
+    <row r="194" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>237</v>
       </c>
@@ -12152,7 +12275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="19.5">
+    <row r="195" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>237</v>
       </c>
@@ -12212,7 +12335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="19.5">
+    <row r="196" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>237</v>
       </c>
@@ -12262,7 +12385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="19.5">
+    <row r="197" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>237</v>
       </c>
@@ -12312,7 +12435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="19.5">
+    <row r="198" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>237</v>
       </c>
@@ -12358,7 +12481,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="19.5">
+    <row r="199" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>237</v>
       </c>
@@ -12404,7 +12527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="19.5">
+    <row r="200" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>237</v>
       </c>
@@ -12450,7 +12573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="19.5">
+    <row r="201" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>237</v>
       </c>
@@ -12496,7 +12619,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="19.5">
+    <row r="202" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>237</v>
       </c>
@@ -12542,7 +12665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="19.5">
+    <row r="203" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>237</v>
       </c>
@@ -12588,7 +12711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="29.25">
+    <row r="204" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>237</v>
       </c>
@@ -12634,7 +12757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="29.25">
+    <row r="205" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>237</v>
       </c>
@@ -12678,7 +12801,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="58.5">
+    <row r="206" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>258</v>
       </c>
@@ -12734,7 +12857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="58.5">
+    <row r="207" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>258</v>
       </c>
@@ -12789,12 +12912,14 @@
       <c r="R207" s="4">
         <v>29.8</v>
       </c>
-      <c r="S207" s="3"/>
+      <c r="S207" s="4">
+        <v>30.4</v>
+      </c>
       <c r="T207" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="58.5">
+    <row r="208" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>258</v>
       </c>
@@ -12852,7 +12977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="58.5">
+    <row r="209" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>258</v>
       </c>
@@ -12912,7 +13037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="58.5">
+    <row r="210" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>258</v>
       </c>
@@ -12972,7 +13097,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="58.5">
+    <row r="211" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>258</v>
       </c>
@@ -13032,7 +13157,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="58.5">
+    <row r="212" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>258</v>
       </c>
@@ -13092,7 +13217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="58.5">
+    <row r="213" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>258</v>
       </c>
@@ -13152,7 +13277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="58.5">
+    <row r="214" spans="1:20" ht="54" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>258</v>
       </c>
@@ -13212,7 +13337,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="39">
+    <row r="215" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>258</v>
       </c>
@@ -13272,7 +13397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="39">
+    <row r="216" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>258</v>
       </c>
@@ -13332,7 +13457,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="39">
+    <row r="217" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>258</v>
       </c>
@@ -13372,7 +13497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="39">
+    <row r="218" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>258</v>
       </c>
@@ -13412,7 +13537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="48.75">
+    <row r="219" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>258</v>
       </c>
@@ -13472,7 +13597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="48.75">
+    <row r="220" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>258</v>
       </c>
@@ -13528,7 +13653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="48.75">
+    <row r="221" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>258</v>
       </c>
@@ -13566,7 +13691,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="29.25">
+    <row r="222" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>258</v>
       </c>
@@ -13622,7 +13747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="29.25">
+    <row r="223" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>258</v>
       </c>
@@ -13670,7 +13795,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="29.25">
+    <row r="224" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>258</v>
       </c>
@@ -13730,7 +13855,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="29.25">
+    <row r="225" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>258</v>
       </c>
@@ -13785,12 +13910,14 @@
       <c r="R225" s="4">
         <v>6.6</v>
       </c>
-      <c r="S225" s="3"/>
+      <c r="S225" s="4">
+        <v>6.6</v>
+      </c>
       <c r="T225" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="29.25">
+    <row r="226" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>258</v>
       </c>
@@ -13850,7 +13977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="29.25">
+    <row r="227" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>258</v>
       </c>
@@ -13892,7 +14019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="29.25">
+    <row r="228" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>258</v>
       </c>
@@ -13938,7 +14065,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="29.25">
+    <row r="229" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>258</v>
       </c>
@@ -13998,7 +14125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="29.25">
+    <row r="230" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>258</v>
       </c>
@@ -14058,7 +14185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="39">
+    <row r="231" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>258</v>
       </c>
@@ -14116,7 +14243,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="39">
+    <row r="232" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>299</v>
       </c>
@@ -14176,7 +14303,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="39">
+    <row r="233" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>299</v>
       </c>
@@ -14236,7 +14363,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="39">
+    <row r="234" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>299</v>
       </c>
@@ -14296,7 +14423,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="39">
+    <row r="235" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>299</v>
       </c>
@@ -14354,7 +14481,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="48.75">
+    <row r="236" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>308</v>
       </c>
@@ -14414,7 +14541,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="48.75">
+    <row r="237" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>308</v>
       </c>
@@ -14474,7 +14601,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="29.25">
+    <row r="238" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>308</v>
       </c>
@@ -14534,7 +14661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="29.25">
+    <row r="239" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>308</v>
       </c>
@@ -14592,7 +14719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="29.25">
+    <row r="240" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>308</v>
       </c>
@@ -14652,7 +14779,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="29.25">
+    <row r="241" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>308</v>
       </c>
@@ -14710,7 +14837,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="29.25">
+    <row r="242" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>308</v>
       </c>
@@ -14770,7 +14897,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="29.25">
+    <row r="243" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>308</v>
       </c>
@@ -14828,7 +14955,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="29.25">
+    <row r="244" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>308</v>
       </c>
@@ -14886,7 +15013,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="19.5">
+    <row r="245" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>308</v>
       </c>
@@ -14946,7 +15073,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="19.5">
+    <row r="246" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>308</v>
       </c>
@@ -14999,12 +15126,14 @@
       <c r="R246" s="4">
         <v>855928.1</v>
       </c>
-      <c r="S246" s="3"/>
+      <c r="S246" s="4">
+        <v>859996.9</v>
+      </c>
       <c r="T246" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="19.5">
+    <row r="247" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>308</v>
       </c>
@@ -15052,7 +15181,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="19.5">
+    <row r="248" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>308</v>
       </c>
@@ -15094,7 +15223,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="146.25">
+    <row r="249" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>308</v>
       </c>
@@ -15132,7 +15261,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="39">
+    <row r="250" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>308</v>
       </c>
@@ -15170,7 +15299,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="78">
+    <row r="251" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>344</v>
       </c>
@@ -15232,7 +15361,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="78">
+    <row r="252" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>344</v>
       </c>
@@ -15294,7 +15423,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="78">
+    <row r="253" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>344</v>
       </c>
@@ -15356,7 +15485,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="78">
+    <row r="254" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>344</v>
       </c>
@@ -15418,7 +15547,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="19.5">
+    <row r="255" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>344</v>
       </c>
@@ -15478,7 +15607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="29.25">
+    <row r="256" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>344</v>
       </c>
@@ -15538,7 +15667,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="39">
+    <row r="257" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>358</v>
       </c>
@@ -15600,7 +15729,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="39">
+    <row r="258" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>358</v>
       </c>
@@ -15655,12 +15784,14 @@
       <c r="R258" s="7">
         <v>0.19900000000000001</v>
       </c>
-      <c r="S258" s="3"/>
+      <c r="S258" s="7">
+        <v>0.19800000000000001</v>
+      </c>
       <c r="T258" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="39">
+    <row r="259" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>358</v>
       </c>
@@ -15715,12 +15846,14 @@
       <c r="R259" s="4">
         <v>30.9</v>
       </c>
-      <c r="S259" s="3"/>
+      <c r="S259" s="4">
+        <v>31</v>
+      </c>
       <c r="T259" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="39">
+    <row r="260" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>358</v>
       </c>
@@ -15780,7 +15913,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="39">
+    <row r="261" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>358</v>
       </c>
@@ -15840,7 +15973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="39">
+    <row r="262" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>358</v>
       </c>
@@ -15900,7 +16033,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="39">
+    <row r="263" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>358</v>
       </c>
@@ -15960,7 +16093,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="39">
+    <row r="264" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>358</v>
       </c>
@@ -16020,7 +16153,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="29.25">
+    <row r="265" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>358</v>
       </c>
@@ -16080,7 +16213,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="29.25">
+    <row r="266" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>358</v>
       </c>
@@ -16140,7 +16273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="29.25">
+    <row r="267" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>374</v>
       </c>
@@ -16202,7 +16335,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="29.25">
+    <row r="268" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>374</v>
       </c>
@@ -16250,7 +16383,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="29.25">
+    <row r="269" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>374</v>
       </c>
@@ -16310,7 +16443,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="29.25">
+    <row r="270" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>374</v>
       </c>
@@ -16370,7 +16503,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="29.25">
+    <row r="271" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>374</v>
       </c>
@@ -16430,7 +16563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="29.25">
+    <row r="272" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>374</v>
       </c>
@@ -16490,7 +16623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="29.25">
+    <row r="273" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>374</v>
       </c>
@@ -16550,7 +16683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="29.25">
+    <row r="274" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>374</v>
       </c>
@@ -16610,7 +16743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="29.25">
+    <row r="275" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>374</v>
       </c>
@@ -16670,7 +16803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="29.25">
+    <row r="276" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>374</v>
       </c>
@@ -16730,7 +16863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="29.25">
+    <row r="277" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>374</v>
       </c>
@@ -16790,7 +16923,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="29.25">
+    <row r="278" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>374</v>
       </c>
@@ -16850,7 +16983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="29.25">
+    <row r="279" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>374</v>
       </c>
@@ -16910,7 +17043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="29.25">
+    <row r="280" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>374</v>
       </c>
@@ -16970,7 +17103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="29.25">
+    <row r="281" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>374</v>
       </c>
@@ -17030,7 +17163,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="29.25">
+    <row r="282" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>374</v>
       </c>
@@ -17090,7 +17223,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="29.25">
+    <row r="283" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>374</v>
       </c>
@@ -17150,7 +17283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="29.25">
+    <row r="284" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>374</v>
       </c>
@@ -17210,7 +17343,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="29.25">
+    <row r="285" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>374</v>
       </c>
@@ -17270,7 +17403,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="29.25">
+    <row r="286" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>374</v>
       </c>
@@ -17330,7 +17463,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="29.25">
+    <row r="287" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>374</v>
       </c>
@@ -17390,7 +17523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="29.25">
+    <row r="288" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>374</v>
       </c>
@@ -17450,7 +17583,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="29.25">
+    <row r="289" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>374</v>
       </c>
@@ -17505,12 +17638,14 @@
       <c r="R289" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="S289" s="3"/>
+      <c r="S289" s="4">
+        <v>4</v>
+      </c>
       <c r="T289" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="39">
+    <row r="290" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>388</v>
       </c>
@@ -17572,7 +17707,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="39">
+    <row r="291" spans="1:20" ht="36" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>388</v>
       </c>
@@ -17634,7 +17769,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="78">
+    <row r="292" spans="1:20" ht="72" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>388</v>
       </c>
@@ -17689,12 +17824,14 @@
       <c r="R292" s="5">
         <v>0.15</v>
       </c>
-      <c r="S292" s="3"/>
+      <c r="S292" s="5">
+        <v>0.53</v>
+      </c>
       <c r="T292" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="29.25">
+    <row r="293" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>388</v>
       </c>
@@ -17748,7 +17885,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="29.25">
+    <row r="294" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>388</v>
       </c>
@@ -17797,12 +17934,14 @@
       <c r="R294" s="5">
         <v>3.65</v>
       </c>
-      <c r="S294" s="3"/>
+      <c r="S294" s="5">
+        <v>9.59</v>
+      </c>
       <c r="T294" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="39">
+    <row r="295" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>388</v>
       </c>
@@ -17848,7 +17987,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="29.25">
+    <row r="296" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>388</v>
       </c>
@@ -17902,7 +18041,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="29.25">
+    <row r="297" spans="1:20" ht="27" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>388</v>
       </c>
@@ -17950,9 +18089,9 @@
         <v>403</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="0" hidden="1" customHeight="1"/>
-    <row r="299" spans="1:20" ht="18" customHeight="1"/>
-    <row r="300" spans="1:20" ht="17.100000000000001" customHeight="1">
+    <row r="298" spans="1:20" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="1:20" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="10" t="s">
         <v>408</v>
       </c>
@@ -17969,7 +18108,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="63" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe 06.02.2024 - aktualizacja plików excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sidwab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dregerj\Documents\SDG\sdg_git_produkcja\sdg-indicators-pl\assets\excel\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="410">
   <si>
     <t>sdg.gov.pl/en</t>
   </si>
@@ -661,7 +661,7 @@
     <t>Promotion of stable forms of employment</t>
   </si>
   <si>
-    <t>8.4.a Percentage of employees hired on the basis of employment contract in relation to the number of persons employed in national economy</t>
+    <t>8.4.a Percentage of paid employees in relation to the number of persons employed in national economy.</t>
   </si>
   <si>
     <t>Work activation of young people, women, persons aged 50+ , long-term unemployed as well as persons with disabilities</t>
@@ -1243,7 +1243,16 @@
     <t>17.6.a Number of National Revenue Administration experts participating in conferences and training activities</t>
   </si>
   <si>
-    <t>Last update: 09-01-2024, 09:46</t>
+    <t>Increasing policy coherence for sustainable development</t>
+  </si>
+  <si>
+    <t>17.7.a Number of participants who completed e-learning courses on issues related to sustainable development</t>
+  </si>
+  <si>
+    <t>The Ministry of Economic Development and Technology / The Chancellery of the  Prime Minister</t>
+  </si>
+  <si>
+    <t>Last update: 07-02-2024, 08:56</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1265,7 @@
     <numFmt numFmtId="166" formatCode="[$-10809]0;\-0;0"/>
     <numFmt numFmtId="167" formatCode="[$-10809]0.000;\-0.000;0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1783,14 +1792,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U298"/>
+  <dimension ref="A1:U300"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
@@ -1804,17 +1813,17 @@
     <col min="23" max="23" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="36" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="25.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="29.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1930,13 +1939,15 @@
       <c r="R4" s="4">
         <v>2.8</v>
       </c>
-      <c r="S4" s="3"/>
+      <c r="S4" s="4">
+        <v>2.8</v>
+      </c>
       <c r="T4" s="3"/>
       <c r="U4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="29.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1987,13 +1998,15 @@
       <c r="R5" s="4">
         <v>121.5</v>
       </c>
-      <c r="S5" s="3"/>
+      <c r="S5" s="4">
+        <v>132.5</v>
+      </c>
       <c r="T5" s="3"/>
       <c r="U5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="29.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="29.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -2113,7 +2126,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="29.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -2172,7 +2185,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -2235,7 +2248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2298,7 +2311,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2361,7 +2374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="39">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -2422,7 +2435,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="29.25">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
@@ -2451,7 +2464,7 @@
         <v>0.04</v>
       </c>
       <c r="J13" s="5">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="K13" s="5">
         <v>0.06</v>
@@ -2477,13 +2490,15 @@
       <c r="R13" s="5">
         <v>0.06</v>
       </c>
-      <c r="S13" s="3"/>
+      <c r="S13" s="5">
+        <v>0.05</v>
+      </c>
       <c r="T13" s="3"/>
       <c r="U13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="29.25">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
@@ -2542,7 +2557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="29.25">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -2601,7 +2616,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="29.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -2660,7 +2675,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="39">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -2723,7 +2738,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="29.25">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -2784,7 +2799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="29.25">
       <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
@@ -2845,7 +2860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="19.5">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
@@ -2888,7 +2903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="19.5">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -2931,7 +2946,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="19.5">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2974,7 +2989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="19.5">
       <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
@@ -3017,7 +3032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="19.5">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -3064,7 +3079,7 @@
         <v>59.8</v>
       </c>
       <c r="P24" s="4">
-        <v>59.8</v>
+        <v>59.7</v>
       </c>
       <c r="Q24" s="4">
         <v>59.2</v>
@@ -3072,13 +3087,15 @@
       <c r="R24" s="4">
         <v>59.1</v>
       </c>
-      <c r="S24" s="3"/>
+      <c r="S24" s="4">
+        <v>60.1</v>
+      </c>
       <c r="T24" s="3"/>
       <c r="U24" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="19.5">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -3133,13 +3150,15 @@
       <c r="R25" s="4">
         <v>63.1</v>
       </c>
-      <c r="S25" s="3"/>
+      <c r="S25" s="4">
+        <v>63.7</v>
+      </c>
       <c r="T25" s="3"/>
       <c r="U25" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="19.5">
       <c r="A26" s="2" t="s">
         <v>64</v>
       </c>
@@ -3200,7 +3219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="19.5">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -3261,7 +3280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="19.5">
       <c r="A28" s="2" t="s">
         <v>64</v>
       </c>
@@ -3322,7 +3341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="19.5">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
@@ -3383,7 +3402,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="19.5">
       <c r="A30" s="2" t="s">
         <v>64</v>
       </c>
@@ -3444,7 +3463,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="19.5">
       <c r="A31" s="2" t="s">
         <v>64</v>
       </c>
@@ -3505,7 +3524,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="19.5">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -3566,7 +3585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="19.5">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -3627,7 +3646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="19.5">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -3688,7 +3707,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="19.5">
       <c r="A35" s="2" t="s">
         <v>64</v>
       </c>
@@ -3749,7 +3768,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="19.5">
       <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
@@ -3810,7 +3829,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="19.5">
       <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
@@ -3871,7 +3890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="19.5">
       <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
@@ -3932,7 +3951,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="19.5">
       <c r="A39" s="2" t="s">
         <v>64</v>
       </c>
@@ -3993,7 +4012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="19.5">
       <c r="A40" s="2" t="s">
         <v>64</v>
       </c>
@@ -4054,7 +4073,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="19.5">
       <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
@@ -4115,7 +4134,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="19.5">
       <c r="A42" s="2" t="s">
         <v>64</v>
       </c>
@@ -4176,7 +4195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="19.5">
       <c r="A43" s="2" t="s">
         <v>64</v>
       </c>
@@ -4237,7 +4256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="19.5">
       <c r="A44" s="2" t="s">
         <v>64</v>
       </c>
@@ -4298,7 +4317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="19.5">
       <c r="A45" s="2" t="s">
         <v>64</v>
       </c>
@@ -4359,7 +4378,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="19.5">
       <c r="A46" s="2" t="s">
         <v>64</v>
       </c>
@@ -4396,13 +4415,15 @@
       <c r="R46" s="4">
         <v>34.299999999999997</v>
       </c>
-      <c r="S46" s="3"/>
+      <c r="S46" s="4">
+        <v>34.799999999999997</v>
+      </c>
       <c r="T46" s="3"/>
       <c r="U46" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="19.5">
       <c r="A47" s="2" t="s">
         <v>64</v>
       </c>
@@ -4439,13 +4460,15 @@
       <c r="R47" s="4">
         <v>64.099999999999994</v>
       </c>
-      <c r="S47" s="3"/>
+      <c r="S47" s="4">
+        <v>63.8</v>
+      </c>
       <c r="T47" s="3"/>
       <c r="U47" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="19.5">
       <c r="A48" s="2" t="s">
         <v>64</v>
       </c>
@@ -4488,7 +4511,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="19.5">
       <c r="A49" s="2" t="s">
         <v>64</v>
       </c>
@@ -4531,7 +4554,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="19.5">
       <c r="A50" s="2" t="s">
         <v>64</v>
       </c>
@@ -4574,7 +4597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="19.5">
       <c r="A51" s="2" t="s">
         <v>64</v>
       </c>
@@ -4617,7 +4640,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="19.5">
       <c r="A52" s="2" t="s">
         <v>64</v>
       </c>
@@ -4660,7 +4683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="19.5">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
@@ -4703,7 +4726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="19.5">
       <c r="A54" s="2" t="s">
         <v>64</v>
       </c>
@@ -4746,7 +4769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="19.5">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -4789,7 +4812,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="19.5">
       <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
@@ -4832,7 +4855,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="19.5">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -4875,7 +4898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="19.5">
       <c r="A58" s="2" t="s">
         <v>64</v>
       </c>
@@ -4916,7 +4939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="19.5">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -4957,7 +4980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="19.5">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -4998,7 +5021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="19.5">
       <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
@@ -5061,7 +5084,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="29.25">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
@@ -5116,7 +5139,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="29.25">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
@@ -5171,7 +5194,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="29.25">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -5226,7 +5249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="29.25">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
@@ -5271,7 +5294,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="48.75">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -5334,7 +5357,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="39">
       <c r="A67" s="2" t="s">
         <v>98</v>
       </c>
@@ -5397,7 +5420,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="39">
       <c r="A68" s="2" t="s">
         <v>98</v>
       </c>
@@ -5446,7 +5469,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="48.75">
       <c r="A69" s="2" t="s">
         <v>98</v>
       </c>
@@ -5485,13 +5508,15 @@
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
-      <c r="S69" s="3"/>
+      <c r="S69" s="4">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="T69" s="3"/>
       <c r="U69" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="48.75">
       <c r="A70" s="2" t="s">
         <v>98</v>
       </c>
@@ -5530,13 +5555,15 @@
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
+      <c r="S70" s="4">
+        <v>9.4</v>
+      </c>
       <c r="T70" s="3"/>
       <c r="U70" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="48.75">
       <c r="A71" s="2" t="s">
         <v>98</v>
       </c>
@@ -5575,13 +5602,15 @@
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
-      <c r="S71" s="3"/>
+      <c r="S71" s="4">
+        <v>22.3</v>
+      </c>
       <c r="T71" s="3"/>
       <c r="U71" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="48.75">
       <c r="A72" s="2" t="s">
         <v>98</v>
       </c>
@@ -5620,13 +5649,15 @@
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
-      <c r="S72" s="3"/>
+      <c r="S72" s="4">
+        <v>23</v>
+      </c>
       <c r="T72" s="3"/>
       <c r="U72" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="48.75">
       <c r="A73" s="2" t="s">
         <v>98</v>
       </c>
@@ -5665,13 +5696,15 @@
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
-      <c r="S73" s="3"/>
+      <c r="S73" s="4">
+        <v>77.8</v>
+      </c>
       <c r="T73" s="3"/>
       <c r="U73" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="48.75">
       <c r="A74" s="2" t="s">
         <v>98</v>
       </c>
@@ -5710,13 +5743,15 @@
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
       <c r="R74" s="3"/>
-      <c r="S74" s="3"/>
+      <c r="S74" s="4">
+        <v>77</v>
+      </c>
       <c r="T74" s="3"/>
       <c r="U74" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="29.25">
       <c r="A75" s="2" t="s">
         <v>98</v>
       </c>
@@ -5779,7 +5814,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="29.25">
       <c r="A76" s="2" t="s">
         <v>98</v>
       </c>
@@ -5842,7 +5877,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="29.25">
       <c r="A77" s="2" t="s">
         <v>98</v>
       </c>
@@ -5905,7 +5940,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="39">
       <c r="A78" s="2" t="s">
         <v>98</v>
       </c>
@@ -5968,7 +6003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="39">
       <c r="A79" s="2" t="s">
         <v>98</v>
       </c>
@@ -6031,7 +6066,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="39">
       <c r="A80" s="2" t="s">
         <v>98</v>
       </c>
@@ -6094,7 +6129,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="39">
       <c r="A81" s="2" t="s">
         <v>98</v>
       </c>
@@ -6157,7 +6192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="39">
       <c r="A82" s="2" t="s">
         <v>98</v>
       </c>
@@ -6220,7 +6255,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="39">
       <c r="A83" s="2" t="s">
         <v>98</v>
       </c>
@@ -6283,7 +6318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="39">
       <c r="A84" s="2" t="s">
         <v>98</v>
       </c>
@@ -6346,7 +6381,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" ht="39">
       <c r="A85" s="2" t="s">
         <v>98</v>
       </c>
@@ -6409,7 +6444,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" ht="39">
       <c r="A86" s="2" t="s">
         <v>98</v>
       </c>
@@ -6472,7 +6507,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" ht="39">
       <c r="A87" s="2" t="s">
         <v>98</v>
       </c>
@@ -6535,7 +6570,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" ht="39">
       <c r="A88" s="2" t="s">
         <v>98</v>
       </c>
@@ -6598,7 +6633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" ht="29.25">
       <c r="A89" s="2" t="s">
         <v>98</v>
       </c>
@@ -6639,7 +6674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" ht="29.25">
       <c r="A90" s="2" t="s">
         <v>98</v>
       </c>
@@ -6678,7 +6713,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" ht="29.25">
       <c r="A91" s="2" t="s">
         <v>98</v>
       </c>
@@ -6717,7 +6752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" ht="29.25">
       <c r="A92" s="2" t="s">
         <v>98</v>
       </c>
@@ -6756,7 +6791,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" ht="29.25">
       <c r="A93" s="2" t="s">
         <v>98</v>
       </c>
@@ -6795,7 +6830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" ht="29.25">
       <c r="A94" s="2" t="s">
         <v>98</v>
       </c>
@@ -6834,7 +6869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" ht="29.25">
       <c r="A95" s="2" t="s">
         <v>98</v>
       </c>
@@ -6873,7 +6908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" ht="19.5">
       <c r="A96" s="2" t="s">
         <v>98</v>
       </c>
@@ -6907,12 +6942,14 @@
         <v>21</v>
       </c>
       <c r="S96" s="3"/>
-      <c r="T96" s="3"/>
+      <c r="T96" s="6">
+        <v>20</v>
+      </c>
       <c r="U96" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" ht="19.5">
       <c r="A97" s="2" t="s">
         <v>98</v>
       </c>
@@ -6946,12 +6983,14 @@
         <v>20</v>
       </c>
       <c r="S97" s="3"/>
-      <c r="T97" s="3"/>
+      <c r="T97" s="6">
+        <v>19</v>
+      </c>
       <c r="U97" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" ht="19.5">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -6985,12 +7024,14 @@
         <v>22</v>
       </c>
       <c r="S98" s="3"/>
-      <c r="T98" s="3"/>
+      <c r="T98" s="6">
+        <v>21</v>
+      </c>
       <c r="U98" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" ht="19.5">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
@@ -7024,12 +7065,14 @@
         <v>23</v>
       </c>
       <c r="S99" s="3"/>
-      <c r="T99" s="3"/>
+      <c r="T99" s="6">
+        <v>26</v>
+      </c>
       <c r="U99" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" ht="19.5">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
@@ -7063,12 +7106,14 @@
         <v>21</v>
       </c>
       <c r="S100" s="3"/>
-      <c r="T100" s="3"/>
+      <c r="T100" s="6">
+        <v>12</v>
+      </c>
       <c r="U100" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" ht="19.5">
       <c r="A101" s="2" t="s">
         <v>98</v>
       </c>
@@ -7102,12 +7147,14 @@
         <v>36</v>
       </c>
       <c r="S101" s="3"/>
-      <c r="T101" s="3"/>
+      <c r="T101" s="6">
+        <v>31</v>
+      </c>
       <c r="U101" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" ht="19.5">
       <c r="A102" s="2" t="s">
         <v>98</v>
       </c>
@@ -7141,12 +7188,14 @@
         <v>34</v>
       </c>
       <c r="S102" s="3"/>
-      <c r="T102" s="3"/>
+      <c r="T102" s="6">
+        <v>35</v>
+      </c>
       <c r="U102" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" ht="19.5">
       <c r="A103" s="2" t="s">
         <v>98</v>
       </c>
@@ -7180,12 +7229,14 @@
         <v>28</v>
       </c>
       <c r="S103" s="3"/>
-      <c r="T103" s="3"/>
+      <c r="T103" s="6">
+        <v>27</v>
+      </c>
       <c r="U103" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" ht="19.5">
       <c r="A104" s="2" t="s">
         <v>98</v>
       </c>
@@ -7219,12 +7270,14 @@
         <v>17</v>
       </c>
       <c r="S104" s="3"/>
-      <c r="T104" s="3"/>
+      <c r="T104" s="6">
+        <v>18</v>
+      </c>
       <c r="U104" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" ht="19.5">
       <c r="A105" s="2" t="s">
         <v>98</v>
       </c>
@@ -7258,12 +7311,14 @@
         <v>8</v>
       </c>
       <c r="S105" s="3"/>
-      <c r="T105" s="3"/>
+      <c r="T105" s="6">
+        <v>9</v>
+      </c>
       <c r="U105" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" ht="19.5">
       <c r="A106" s="2" t="s">
         <v>98</v>
       </c>
@@ -7297,12 +7352,14 @@
         <v>3</v>
       </c>
       <c r="S106" s="3"/>
-      <c r="T106" s="3"/>
+      <c r="T106" s="6">
+        <v>3</v>
+      </c>
       <c r="U106" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" ht="19.5">
       <c r="A107" s="2" t="s">
         <v>98</v>
       </c>
@@ -7336,12 +7393,14 @@
         <v>19</v>
       </c>
       <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
+      <c r="T107" s="6">
+        <v>12</v>
+      </c>
       <c r="U107" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" ht="19.5">
       <c r="A108" s="2" t="s">
         <v>98</v>
       </c>
@@ -7375,12 +7434,14 @@
         <v>11</v>
       </c>
       <c r="S108" s="3"/>
-      <c r="T108" s="3"/>
+      <c r="T108" s="6">
+        <v>11</v>
+      </c>
       <c r="U108" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="19.5">
       <c r="A109" s="2" t="s">
         <v>98</v>
       </c>
@@ -7414,12 +7475,14 @@
         <v>42</v>
       </c>
       <c r="S109" s="3"/>
-      <c r="T109" s="3"/>
+      <c r="T109" s="6">
+        <v>42</v>
+      </c>
       <c r="U109" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" ht="19.5">
       <c r="A110" s="2" t="s">
         <v>98</v>
       </c>
@@ -7453,12 +7516,14 @@
         <v>25</v>
       </c>
       <c r="S110" s="3"/>
-      <c r="T110" s="3"/>
+      <c r="T110" s="6">
+        <v>26</v>
+      </c>
       <c r="U110" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" ht="19.5">
       <c r="A111" s="2" t="s">
         <v>98</v>
       </c>
@@ -7492,12 +7557,14 @@
         <v>26</v>
       </c>
       <c r="S111" s="3"/>
-      <c r="T111" s="3"/>
+      <c r="T111" s="6">
+        <v>26</v>
+      </c>
       <c r="U111" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" ht="19.5">
       <c r="A112" s="2" t="s">
         <v>98</v>
       </c>
@@ -7531,12 +7598,14 @@
         <v>12</v>
       </c>
       <c r="S112" s="3"/>
-      <c r="T112" s="3"/>
+      <c r="T112" s="6">
+        <v>15</v>
+      </c>
       <c r="U112" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" ht="19.5">
       <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
@@ -7570,12 +7639,14 @@
         <v>12</v>
       </c>
       <c r="S113" s="3"/>
-      <c r="T113" s="3"/>
+      <c r="T113" s="6">
+        <v>10</v>
+      </c>
       <c r="U113" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" ht="19.5">
       <c r="A114" s="2" t="s">
         <v>147</v>
       </c>
@@ -7628,15 +7699,17 @@
         <v>4.8</v>
       </c>
       <c r="R114" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="S114" s="3"/>
+        <v>6.4</v>
+      </c>
+      <c r="S114" s="4">
+        <v>7.9</v>
+      </c>
       <c r="T114" s="3"/>
       <c r="U114" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" ht="19.5">
       <c r="A115" s="2" t="s">
         <v>147</v>
       </c>
@@ -7699,7 +7772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" ht="19.5">
       <c r="A116" s="2" t="s">
         <v>147</v>
       </c>
@@ -7762,7 +7835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" ht="19.5">
       <c r="A117" s="2" t="s">
         <v>147</v>
       </c>
@@ -7825,7 +7898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" ht="19.5">
       <c r="A118" s="2" t="s">
         <v>147</v>
       </c>
@@ -7874,7 +7947,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" ht="39">
       <c r="A119" s="2" t="s">
         <v>147</v>
       </c>
@@ -7923,7 +7996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" ht="19.5">
       <c r="A120" s="2" t="s">
         <v>147</v>
       </c>
@@ -7972,7 +8045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" ht="39">
       <c r="A121" s="2" t="s">
         <v>147</v>
       </c>
@@ -8021,7 +8094,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="122" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" ht="39">
       <c r="A122" s="2" t="s">
         <v>147</v>
       </c>
@@ -8070,7 +8143,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" ht="39">
       <c r="A123" s="2" t="s">
         <v>147</v>
       </c>
@@ -8119,7 +8192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" ht="39">
       <c r="A124" s="2" t="s">
         <v>147</v>
       </c>
@@ -8168,7 +8241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="125" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:21" ht="19.5">
       <c r="A125" s="2" t="s">
         <v>147</v>
       </c>
@@ -8229,7 +8302,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="126" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:21" ht="19.5">
       <c r="A126" s="2" t="s">
         <v>147</v>
       </c>
@@ -8288,7 +8361,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="127" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:21" ht="19.5">
       <c r="A127" s="2" t="s">
         <v>147</v>
       </c>
@@ -8347,7 +8420,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="128" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:21" ht="29.25">
       <c r="A128" s="2" t="s">
         <v>147</v>
       </c>
@@ -8410,7 +8483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="129" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:21" ht="29.25">
       <c r="A129" s="2" t="s">
         <v>147</v>
       </c>
@@ -8473,7 +8546,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:21" ht="29.25">
       <c r="A130" s="2" t="s">
         <v>147</v>
       </c>
@@ -8536,7 +8609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:21" ht="29.25">
       <c r="A131" s="2" t="s">
         <v>165</v>
       </c>
@@ -8597,7 +8670,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:21" ht="29.25">
       <c r="A132" s="2" t="s">
         <v>165</v>
       </c>
@@ -8652,13 +8725,15 @@
       <c r="R132" s="4">
         <v>0.5</v>
       </c>
-      <c r="S132" s="3"/>
+      <c r="S132" s="4">
+        <v>0.3</v>
+      </c>
       <c r="T132" s="3"/>
       <c r="U132" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:21" ht="39">
       <c r="A133" s="2" t="s">
         <v>165</v>
       </c>
@@ -8721,7 +8796,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:21" ht="39">
       <c r="A134" s="2" t="s">
         <v>165</v>
       </c>
@@ -8784,7 +8859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:21" ht="39">
       <c r="A135" s="2" t="s">
         <v>165</v>
       </c>
@@ -8847,7 +8922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:21" ht="39">
       <c r="A136" s="2" t="s">
         <v>165</v>
       </c>
@@ -8866,49 +8941,51 @@
       <c r="F136" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G136" s="5">
-        <v>65.73</v>
-      </c>
-      <c r="H136" s="5">
-        <v>64.760000000000005</v>
-      </c>
-      <c r="I136" s="5">
-        <v>67.349999999999994</v>
-      </c>
-      <c r="J136" s="5">
-        <v>69.77</v>
-      </c>
-      <c r="K136" s="5">
-        <v>70.48</v>
-      </c>
-      <c r="L136" s="5">
+      <c r="G136" s="4">
+        <v>65.7</v>
+      </c>
+      <c r="H136" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="I136" s="4">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="J136" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="K136" s="4">
+        <v>70.5</v>
+      </c>
+      <c r="L136" s="4">
         <v>70.900000000000006</v>
       </c>
-      <c r="M136" s="5">
-        <v>71.430000000000007</v>
-      </c>
-      <c r="N136" s="5">
-        <v>72.52</v>
-      </c>
-      <c r="O136" s="5">
-        <v>73.17</v>
-      </c>
-      <c r="P136" s="5">
-        <v>73.930000000000007</v>
-      </c>
-      <c r="Q136" s="5">
-        <v>73.319999999999993</v>
-      </c>
-      <c r="R136" s="5">
-        <v>72.849999999999994</v>
-      </c>
-      <c r="S136" s="3"/>
+      <c r="M136" s="4">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="N136" s="4">
+        <v>72.5</v>
+      </c>
+      <c r="O136" s="4">
+        <v>73.2</v>
+      </c>
+      <c r="P136" s="4">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="Q136" s="4">
+        <v>73.3</v>
+      </c>
+      <c r="R136" s="4">
+        <v>72.8</v>
+      </c>
+      <c r="S136" s="4">
+        <v>76.3</v>
+      </c>
       <c r="T136" s="3"/>
       <c r="U136" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:21" ht="29.25">
       <c r="A137" s="2" t="s">
         <v>174</v>
       </c>
@@ -8967,7 +9044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:21" ht="29.25">
       <c r="A138" s="2" t="s">
         <v>174</v>
       </c>
@@ -9028,7 +9105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:21" ht="29.25">
       <c r="A139" s="2" t="s">
         <v>174</v>
       </c>
@@ -9089,7 +9166,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:21" ht="19.5">
       <c r="A140" s="2" t="s">
         <v>174</v>
       </c>
@@ -9150,7 +9227,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:21" ht="39">
       <c r="A141" s="2" t="s">
         <v>186</v>
       </c>
@@ -9211,7 +9288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:21" ht="39">
       <c r="A142" s="2" t="s">
         <v>186</v>
       </c>
@@ -9266,13 +9343,15 @@
       <c r="R142" s="5">
         <v>1.58</v>
       </c>
-      <c r="S142" s="3"/>
+      <c r="S142" s="5">
+        <v>1.82</v>
+      </c>
       <c r="T142" s="3"/>
       <c r="U142" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:21" ht="39">
       <c r="A143" s="2" t="s">
         <v>186</v>
       </c>
@@ -9329,7 +9408,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:21" ht="29.25">
       <c r="A144" s="2" t="s">
         <v>186</v>
       </c>
@@ -9382,7 +9461,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:21" ht="29.25">
       <c r="A145" s="2" t="s">
         <v>186</v>
       </c>
@@ -9445,7 +9524,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:21" ht="29.25">
       <c r="A146" s="2" t="s">
         <v>186</v>
       </c>
@@ -9508,7 +9587,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:21" ht="29.25">
       <c r="A147" s="2" t="s">
         <v>186</v>
       </c>
@@ -9571,7 +9650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:21" ht="29.25">
       <c r="A148" s="2" t="s">
         <v>186</v>
       </c>
@@ -9634,7 +9713,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:21" ht="29.25">
       <c r="A149" s="2" t="s">
         <v>186</v>
       </c>
@@ -9697,7 +9776,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:21" ht="29.25">
       <c r="A150" s="2" t="s">
         <v>186</v>
       </c>
@@ -9760,7 +9839,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="151" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:21" ht="29.25">
       <c r="A151" s="2" t="s">
         <v>186</v>
       </c>
@@ -9823,7 +9902,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="152" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:21" ht="29.25">
       <c r="A152" s="2" t="s">
         <v>186</v>
       </c>
@@ -9886,7 +9965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:21" ht="29.25">
       <c r="A153" s="2" t="s">
         <v>186</v>
       </c>
@@ -9949,7 +10028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="154" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:21" ht="29.25">
       <c r="A154" s="2" t="s">
         <v>186</v>
       </c>
@@ -10012,7 +10091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="155" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:21" ht="29.25">
       <c r="A155" s="2" t="s">
         <v>186</v>
       </c>
@@ -10075,7 +10154,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:21" ht="29.25">
       <c r="A156" s="2" t="s">
         <v>186</v>
       </c>
@@ -10138,7 +10217,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="157" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:21" ht="29.25">
       <c r="A157" s="2" t="s">
         <v>186</v>
       </c>
@@ -10201,7 +10280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:21" ht="29.25">
       <c r="A158" s="2" t="s">
         <v>186</v>
       </c>
@@ -10264,7 +10343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="159" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:21" ht="29.25">
       <c r="A159" s="2" t="s">
         <v>186</v>
       </c>
@@ -10327,7 +10406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:21" ht="29.25">
       <c r="A160" s="2" t="s">
         <v>186</v>
       </c>
@@ -10390,7 +10469,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="161" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" ht="29.25">
       <c r="A161" s="2" t="s">
         <v>186</v>
       </c>
@@ -10453,7 +10532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" ht="48.75">
       <c r="A162" s="2" t="s">
         <v>186</v>
       </c>
@@ -10516,7 +10595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" ht="29.25">
       <c r="A163" s="2" t="s">
         <v>186</v>
       </c>
@@ -10577,7 +10656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" ht="29.25">
       <c r="A164" s="2" t="s">
         <v>186</v>
       </c>
@@ -10638,7 +10717,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" ht="29.25">
       <c r="A165" s="2" t="s">
         <v>186</v>
       </c>
@@ -10699,7 +10778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" ht="29.25">
       <c r="A166" s="2" t="s">
         <v>186</v>
       </c>
@@ -10762,7 +10841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" ht="29.25">
       <c r="A167" s="2" t="s">
         <v>186</v>
       </c>
@@ -10825,7 +10904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="168" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" ht="29.25">
       <c r="A168" s="2" t="s">
         <v>186</v>
       </c>
@@ -10888,7 +10967,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="169" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" ht="29.25">
       <c r="A169" s="2" t="s">
         <v>186</v>
       </c>
@@ -10951,7 +11030,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" ht="29.25">
       <c r="A170" s="2" t="s">
         <v>186</v>
       </c>
@@ -11014,7 +11093,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="171" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" ht="29.25">
       <c r="A171" s="2" t="s">
         <v>186</v>
       </c>
@@ -11077,7 +11156,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="172" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" ht="29.25">
       <c r="A172" s="2" t="s">
         <v>186</v>
       </c>
@@ -11140,7 +11219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="173" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" ht="29.25">
       <c r="A173" s="2" t="s">
         <v>186</v>
       </c>
@@ -11203,7 +11282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="174" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" ht="29.25">
       <c r="A174" s="2" t="s">
         <v>186</v>
       </c>
@@ -11266,7 +11345,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="175" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" ht="29.25">
       <c r="A175" s="2" t="s">
         <v>186</v>
       </c>
@@ -11329,7 +11408,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="176" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" ht="29.25">
       <c r="A176" s="2" t="s">
         <v>186</v>
       </c>
@@ -11392,7 +11471,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="177" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" ht="29.25">
       <c r="A177" s="2" t="s">
         <v>186</v>
       </c>
@@ -11455,7 +11534,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="178" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" ht="29.25">
       <c r="A178" s="2" t="s">
         <v>186</v>
       </c>
@@ -11518,7 +11597,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="179" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" ht="29.25">
       <c r="A179" s="2" t="s">
         <v>186</v>
       </c>
@@ -11581,7 +11660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="180" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" ht="29.25">
       <c r="A180" s="2" t="s">
         <v>186</v>
       </c>
@@ -11644,7 +11723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="181" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" ht="29.25">
       <c r="A181" s="2" t="s">
         <v>186</v>
       </c>
@@ -11707,7 +11786,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="182" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" ht="29.25">
       <c r="A182" s="2" t="s">
         <v>186</v>
       </c>
@@ -11770,7 +11849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="183" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" ht="29.25">
       <c r="A183" s="2" t="s">
         <v>186</v>
       </c>
@@ -11831,7 +11910,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="184" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" ht="29.25">
       <c r="A184" s="2" t="s">
         <v>186</v>
       </c>
@@ -11892,7 +11971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="185" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" ht="29.25">
       <c r="A185" s="2" t="s">
         <v>186</v>
       </c>
@@ -11953,7 +12032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="186" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" ht="29.25">
       <c r="A186" s="2" t="s">
         <v>221</v>
       </c>
@@ -12014,7 +12093,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="187" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" ht="29.25">
       <c r="A187" s="2" t="s">
         <v>221</v>
       </c>
@@ -12075,7 +12154,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="188" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" ht="29.25">
       <c r="A188" s="2" t="s">
         <v>221</v>
       </c>
@@ -12130,13 +12209,15 @@
       <c r="R188" s="4">
         <v>16.2</v>
       </c>
-      <c r="S188" s="3"/>
+      <c r="S188" s="4">
+        <v>16.7</v>
+      </c>
       <c r="T188" s="3"/>
       <c r="U188" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" ht="39">
       <c r="A189" s="2" t="s">
         <v>221</v>
       </c>
@@ -12191,7 +12272,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="190" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" ht="29.25">
       <c r="A190" s="2" t="s">
         <v>221</v>
       </c>
@@ -12254,7 +12335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="191" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" ht="19.5">
       <c r="A191" s="2" t="s">
         <v>235</v>
       </c>
@@ -12306,14 +12387,18 @@
       <c r="Q191" s="4">
         <v>12.5</v>
       </c>
-      <c r="R191" s="3"/>
-      <c r="S191" s="3"/>
+      <c r="R191" s="4">
+        <v>12.3</v>
+      </c>
+      <c r="S191" s="4">
+        <v>13.4</v>
+      </c>
       <c r="T191" s="3"/>
       <c r="U191" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="192" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" ht="19.5">
       <c r="A192" s="2" t="s">
         <v>235</v>
       </c>
@@ -12376,7 +12461,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="193" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" ht="19.5">
       <c r="A193" s="2" t="s">
         <v>235</v>
       </c>
@@ -12426,14 +12511,16 @@
       <c r="Q193" s="6">
         <v>-499944</v>
       </c>
-      <c r="R193" s="3"/>
+      <c r="R193" s="6">
+        <v>7406</v>
+      </c>
       <c r="S193" s="3"/>
       <c r="T193" s="3"/>
       <c r="U193" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="194" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" ht="19.5">
       <c r="A194" s="2" t="s">
         <v>235</v>
       </c>
@@ -12488,13 +12575,15 @@
       <c r="R194" s="4">
         <v>26.8</v>
       </c>
-      <c r="S194" s="3"/>
+      <c r="S194" s="4">
+        <v>26.3</v>
+      </c>
       <c r="T194" s="3"/>
       <c r="U194" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="195" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" ht="19.5">
       <c r="A195" s="2" t="s">
         <v>235</v>
       </c>
@@ -12539,13 +12628,15 @@
       <c r="R195" s="4">
         <v>26.2</v>
       </c>
-      <c r="S195" s="3"/>
+      <c r="S195" s="4">
+        <v>25.9</v>
+      </c>
       <c r="T195" s="3"/>
       <c r="U195" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="196" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" ht="19.5">
       <c r="A196" s="2" t="s">
         <v>235</v>
       </c>
@@ -12590,13 +12681,15 @@
       <c r="R196" s="4">
         <v>26.1</v>
       </c>
-      <c r="S196" s="3"/>
+      <c r="S196" s="4">
+        <v>25.6</v>
+      </c>
       <c r="T196" s="3"/>
       <c r="U196" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="197" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" ht="19.5">
       <c r="A197" s="2" t="s">
         <v>235</v>
       </c>
@@ -12643,7 +12736,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="198" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" ht="19.5">
       <c r="A198" s="2" t="s">
         <v>235</v>
       </c>
@@ -12690,7 +12783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="199" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" ht="19.5">
       <c r="A199" s="2" t="s">
         <v>235</v>
       </c>
@@ -12737,7 +12830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="200" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" ht="19.5">
       <c r="A200" s="2" t="s">
         <v>235</v>
       </c>
@@ -12784,7 +12877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="201" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" ht="19.5">
       <c r="A201" s="2" t="s">
         <v>235</v>
       </c>
@@ -12831,7 +12924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="202" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" ht="19.5">
       <c r="A202" s="2" t="s">
         <v>235</v>
       </c>
@@ -12878,7 +12971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="203" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" ht="29.25">
       <c r="A203" s="2" t="s">
         <v>235</v>
       </c>
@@ -12925,7 +13018,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="204" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" ht="29.25">
       <c r="A204" s="2" t="s">
         <v>235</v>
       </c>
@@ -12970,7 +13063,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="205" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" ht="58.5">
       <c r="A205" s="2" t="s">
         <v>256</v>
       </c>
@@ -13027,7 +13120,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="206" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" ht="58.5">
       <c r="A206" s="2" t="s">
         <v>256</v>
       </c>
@@ -13090,7 +13183,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="207" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" ht="58.5">
       <c r="A207" s="2" t="s">
         <v>256</v>
       </c>
@@ -13149,7 +13242,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="208" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" ht="58.5">
       <c r="A208" s="2" t="s">
         <v>256</v>
       </c>
@@ -13212,7 +13305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="209" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:21" ht="58.5">
       <c r="A209" s="2" t="s">
         <v>256</v>
       </c>
@@ -13275,7 +13368,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="210" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:21" ht="58.5">
       <c r="A210" s="2" t="s">
         <v>256</v>
       </c>
@@ -13330,13 +13423,15 @@
       <c r="R210" s="5">
         <v>26.92</v>
       </c>
-      <c r="S210" s="3"/>
+      <c r="S210" s="5">
+        <v>26.72</v>
+      </c>
       <c r="T210" s="3"/>
       <c r="U210" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="211" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:21" ht="58.5">
       <c r="A211" s="2" t="s">
         <v>256</v>
       </c>
@@ -13391,13 +13486,15 @@
       <c r="R211" s="5">
         <v>13.34</v>
       </c>
-      <c r="S211" s="3"/>
+      <c r="S211" s="5">
+        <v>14.15</v>
+      </c>
       <c r="T211" s="3"/>
       <c r="U211" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="212" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:21" ht="58.5">
       <c r="A212" s="2" t="s">
         <v>256</v>
       </c>
@@ -13452,13 +13549,15 @@
       <c r="R212" s="5">
         <v>21.01</v>
       </c>
-      <c r="S212" s="3"/>
+      <c r="S212" s="5">
+        <v>21.07</v>
+      </c>
       <c r="T212" s="3"/>
       <c r="U212" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="213" spans="1:21" ht="54" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:21" ht="58.5">
       <c r="A213" s="2" t="s">
         <v>256</v>
       </c>
@@ -13513,13 +13612,15 @@
       <c r="R213" s="5">
         <v>38.729999999999997</v>
       </c>
-      <c r="S213" s="3"/>
+      <c r="S213" s="5">
+        <v>38.06</v>
+      </c>
       <c r="T213" s="3"/>
       <c r="U213" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="214" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:21" ht="39">
       <c r="A214" s="2" t="s">
         <v>256</v>
       </c>
@@ -13574,13 +13675,15 @@
       <c r="R214" s="4">
         <v>94.6</v>
       </c>
-      <c r="S214" s="3"/>
+      <c r="S214" s="4">
+        <v>95</v>
+      </c>
       <c r="T214" s="3"/>
       <c r="U214" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="215" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:21" ht="39">
       <c r="A215" s="2" t="s">
         <v>256</v>
       </c>
@@ -13635,13 +13738,15 @@
       <c r="R215" s="4">
         <v>96.7</v>
       </c>
-      <c r="S215" s="3"/>
+      <c r="S215" s="4">
+        <v>96.7</v>
+      </c>
       <c r="T215" s="3"/>
       <c r="U215" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="216" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:21" ht="39">
       <c r="A216" s="2" t="s">
         <v>256</v>
       </c>
@@ -13682,7 +13787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="217" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:21" ht="39">
       <c r="A217" s="2" t="s">
         <v>256</v>
       </c>
@@ -13717,13 +13822,15 @@
       <c r="R217" s="4">
         <v>13.5</v>
       </c>
-      <c r="S217" s="3"/>
+      <c r="S217" s="4">
+        <v>13.1</v>
+      </c>
       <c r="T217" s="3"/>
       <c r="U217" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="218" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:21" ht="48.75">
       <c r="A218" s="2" t="s">
         <v>256</v>
       </c>
@@ -13784,7 +13891,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:21" ht="48.75">
       <c r="A219" s="2" t="s">
         <v>256</v>
       </c>
@@ -13843,7 +13950,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:21" ht="48.75">
       <c r="A220" s="2" t="s">
         <v>256</v>
       </c>
@@ -13882,7 +13989,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="221" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:21" ht="29.25">
       <c r="A221" s="2" t="s">
         <v>256</v>
       </c>
@@ -13941,7 +14048,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="222" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:21" ht="29.25">
       <c r="A222" s="2" t="s">
         <v>256</v>
       </c>
@@ -13992,7 +14099,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="223" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:21" ht="29.25">
       <c r="A223" s="2" t="s">
         <v>256</v>
       </c>
@@ -14055,7 +14162,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="224" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:21" ht="29.25">
       <c r="A224" s="2" t="s">
         <v>256</v>
       </c>
@@ -14118,7 +14225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="225" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" ht="29.25">
       <c r="A225" s="2" t="s">
         <v>256</v>
       </c>
@@ -14181,7 +14288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="226" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" ht="29.25">
       <c r="A226" s="2" t="s">
         <v>256</v>
       </c>
@@ -14224,7 +14331,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="227" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" ht="29.25">
       <c r="A227" s="2" t="s">
         <v>256</v>
       </c>
@@ -14265,13 +14372,15 @@
         <v>469607</v>
       </c>
       <c r="R227" s="3"/>
-      <c r="S227" s="3"/>
+      <c r="S227" s="6">
+        <v>457891</v>
+      </c>
       <c r="T227" s="3"/>
       <c r="U227" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="228" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" ht="29.25">
       <c r="A228" s="2" t="s">
         <v>256</v>
       </c>
@@ -14334,7 +14443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="229" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" ht="29.25">
       <c r="A229" s="2" t="s">
         <v>256</v>
       </c>
@@ -14397,7 +14506,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="230" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" ht="39">
       <c r="A230" s="2" t="s">
         <v>256</v>
       </c>
@@ -14458,7 +14567,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="231" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" ht="39">
       <c r="A231" s="2" t="s">
         <v>297</v>
       </c>
@@ -14478,48 +14587,50 @@
         <v>300</v>
       </c>
       <c r="G231" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H231" s="5">
+        <v>0.48</v>
+      </c>
+      <c r="I231" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H231" s="5">
-        <v>0.49</v>
-      </c>
-      <c r="I231" s="5">
-        <v>0.59</v>
-      </c>
       <c r="J231" s="5">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="K231" s="5">
+        <v>0.64</v>
+      </c>
+      <c r="L231" s="5">
+        <v>0.69</v>
+      </c>
+      <c r="M231" s="5">
         <v>0.66</v>
       </c>
-      <c r="L231" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="M231" s="5">
-        <v>0.67</v>
-      </c>
       <c r="N231" s="5">
-        <v>0.69</v>
+        <v>0.68</v>
       </c>
       <c r="O231" s="5">
         <v>0.71</v>
       </c>
       <c r="P231" s="5">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
       <c r="Q231" s="5">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="R231" s="5">
-        <v>0.84</v>
-      </c>
-      <c r="S231" s="3"/>
+        <v>0.85</v>
+      </c>
+      <c r="S231" s="5">
+        <v>0.92</v>
+      </c>
       <c r="T231" s="3"/>
       <c r="U231" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="232" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" ht="39">
       <c r="A232" s="2" t="s">
         <v>297</v>
       </c>
@@ -14539,48 +14650,50 @@
         <v>294</v>
       </c>
       <c r="G232" s="5">
-        <v>16.32</v>
+        <v>16.5</v>
       </c>
       <c r="H232" s="5">
-        <v>20.22</v>
+        <v>20.43</v>
       </c>
       <c r="I232" s="5">
-        <v>17.309999999999999</v>
+        <v>17.52</v>
       </c>
       <c r="J232" s="5">
-        <v>16.510000000000002</v>
+        <v>16.72</v>
       </c>
       <c r="K232" s="5">
-        <v>16.41</v>
+        <v>16.579999999999998</v>
       </c>
       <c r="L232" s="5">
-        <v>16.28</v>
+        <v>16.47</v>
       </c>
       <c r="M232" s="5">
-        <v>16.82</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="N232" s="5">
-        <v>17.829999999999998</v>
+        <v>18.010000000000002</v>
       </c>
       <c r="O232" s="5">
-        <v>18.52</v>
+        <v>18.47</v>
       </c>
       <c r="P232" s="5">
-        <v>17.690000000000001</v>
+        <v>17.59</v>
       </c>
       <c r="Q232" s="5">
-        <v>17.010000000000002</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="R232" s="5">
-        <v>18.02</v>
-      </c>
-      <c r="S232" s="3"/>
+        <v>17.88</v>
+      </c>
+      <c r="S232" s="5">
+        <v>19.350000000000001</v>
+      </c>
       <c r="T232" s="3"/>
       <c r="U232" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="233" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" ht="39">
       <c r="A233" s="2" t="s">
         <v>297</v>
       </c>
@@ -14600,48 +14713,50 @@
         <v>34</v>
       </c>
       <c r="G233" s="4">
-        <v>10.8</v>
+        <v>11.1</v>
       </c>
       <c r="H233" s="4">
+        <v>9.4</v>
+      </c>
+      <c r="I233" s="4">
+        <v>11</v>
+      </c>
+      <c r="J233" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="K233" s="4">
+        <v>13</v>
+      </c>
+      <c r="L233" s="4">
+        <v>11.9</v>
+      </c>
+      <c r="M233" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="N233" s="4">
+        <v>10.4</v>
+      </c>
+      <c r="O233" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="P233" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I233" s="4">
-        <v>10.6</v>
-      </c>
-      <c r="J233" s="4">
-        <v>11.8</v>
-      </c>
-      <c r="K233" s="4">
-        <v>12.6</v>
-      </c>
-      <c r="L233" s="4">
-        <v>11.6</v>
-      </c>
-      <c r="M233" s="4">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="N233" s="4">
-        <v>9.9</v>
-      </c>
-      <c r="O233" s="4">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P233" s="4">
-        <v>10.3</v>
-      </c>
       <c r="Q233" s="4">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="R233" s="4">
         <v>9.1</v>
       </c>
-      <c r="S233" s="3"/>
+      <c r="S233" s="4">
+        <v>8.4</v>
+      </c>
       <c r="T233" s="3"/>
       <c r="U233" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="234" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" ht="39">
       <c r="A234" s="2" t="s">
         <v>297</v>
       </c>
@@ -14700,7 +14815,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="235" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" ht="48.75">
       <c r="A235" s="2" t="s">
         <v>306</v>
       </c>
@@ -14761,7 +14876,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="236" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" ht="48.75">
       <c r="A236" s="2" t="s">
         <v>306</v>
       </c>
@@ -14822,7 +14937,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="237" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" ht="29.25">
       <c r="A237" s="2" t="s">
         <v>306</v>
       </c>
@@ -14883,7 +14998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="238" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" ht="29.25">
       <c r="A238" s="2" t="s">
         <v>306</v>
       </c>
@@ -14942,7 +15057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="239" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" ht="29.25">
       <c r="A239" s="2" t="s">
         <v>306</v>
       </c>
@@ -15005,7 +15120,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="240" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" ht="29.25">
       <c r="A240" s="2" t="s">
         <v>306</v>
       </c>
@@ -15066,7 +15181,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="241" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:21" ht="29.25">
       <c r="A241" s="2" t="s">
         <v>306</v>
       </c>
@@ -15129,7 +15244,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="242" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:21" ht="29.25">
       <c r="A242" s="2" t="s">
         <v>306</v>
       </c>
@@ -15181,14 +15296,16 @@
       <c r="Q242" s="6">
         <v>1820</v>
       </c>
-      <c r="R242" s="3"/>
+      <c r="R242" s="6">
+        <v>2205</v>
+      </c>
       <c r="S242" s="3"/>
       <c r="T242" s="3"/>
       <c r="U242" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="243" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:21" ht="29.25">
       <c r="A243" s="2" t="s">
         <v>306</v>
       </c>
@@ -15247,7 +15364,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="244" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:21" ht="19.5">
       <c r="A244" s="2" t="s">
         <v>306</v>
       </c>
@@ -15308,7 +15425,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="245" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:21" ht="19.5">
       <c r="A245" s="2" t="s">
         <v>306</v>
       </c>
@@ -15369,7 +15486,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="246" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:21" ht="19.5">
       <c r="A246" s="2" t="s">
         <v>306</v>
       </c>
@@ -15418,7 +15535,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="247" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:21" ht="19.5">
       <c r="A247" s="2" t="s">
         <v>306</v>
       </c>
@@ -15463,7 +15580,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="248" spans="1:21" ht="135" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:21" ht="146.25">
       <c r="A248" s="2" t="s">
         <v>306</v>
       </c>
@@ -15502,7 +15619,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="249" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:21" ht="39">
       <c r="A249" s="2" t="s">
         <v>306</v>
       </c>
@@ -15541,7 +15658,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="250" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:21" ht="78">
       <c r="A250" s="2" t="s">
         <v>342</v>
       </c>
@@ -15604,7 +15721,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="251" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:21" ht="78">
       <c r="A251" s="2" t="s">
         <v>342</v>
       </c>
@@ -15667,7 +15784,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="252" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:21" ht="78">
       <c r="A252" s="2" t="s">
         <v>342</v>
       </c>
@@ -15730,7 +15847,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="253" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:21" ht="78">
       <c r="A253" s="2" t="s">
         <v>342</v>
       </c>
@@ -15793,7 +15910,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="254" spans="1:21" ht="18" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:21" ht="19.5">
       <c r="A254" s="2" t="s">
         <v>342</v>
       </c>
@@ -15848,13 +15965,15 @@
       <c r="R254" s="4">
         <v>190.1</v>
       </c>
-      <c r="S254" s="3"/>
+      <c r="S254" s="4">
+        <v>200.8</v>
+      </c>
       <c r="T254" s="3"/>
       <c r="U254" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="255" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:21" ht="29.25">
       <c r="A255" s="2" t="s">
         <v>342</v>
       </c>
@@ -15917,7 +16036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="256" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:21" ht="39">
       <c r="A256" s="2" t="s">
         <v>356</v>
       </c>
@@ -15980,7 +16099,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="257" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:21" ht="39">
       <c r="A257" s="2" t="s">
         <v>356</v>
       </c>
@@ -16043,7 +16162,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="258" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:21" ht="39">
       <c r="A258" s="2" t="s">
         <v>356</v>
       </c>
@@ -16106,7 +16225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="259" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:21" ht="39">
       <c r="A259" s="2" t="s">
         <v>356</v>
       </c>
@@ -16169,7 +16288,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="260" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:21" ht="39">
       <c r="A260" s="2" t="s">
         <v>356</v>
       </c>
@@ -16232,7 +16351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:21" ht="39">
       <c r="A261" s="2" t="s">
         <v>356</v>
       </c>
@@ -16295,7 +16414,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="262" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:21" ht="39">
       <c r="A262" s="2" t="s">
         <v>356</v>
       </c>
@@ -16358,7 +16477,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="263" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:21" ht="39">
       <c r="A263" s="2" t="s">
         <v>356</v>
       </c>
@@ -16377,49 +16496,51 @@
       <c r="F263" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G263" s="5">
-        <v>65.73</v>
-      </c>
-      <c r="H263" s="5">
-        <v>64.760000000000005</v>
-      </c>
-      <c r="I263" s="5">
-        <v>67.349999999999994</v>
-      </c>
-      <c r="J263" s="5">
-        <v>69.77</v>
-      </c>
-      <c r="K263" s="5">
-        <v>70.48</v>
-      </c>
-      <c r="L263" s="5">
+      <c r="G263" s="4">
+        <v>65.7</v>
+      </c>
+      <c r="H263" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="I263" s="4">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="J263" s="4">
+        <v>69.8</v>
+      </c>
+      <c r="K263" s="4">
+        <v>70.5</v>
+      </c>
+      <c r="L263" s="4">
         <v>70.900000000000006</v>
       </c>
-      <c r="M263" s="5">
-        <v>71.430000000000007</v>
-      </c>
-      <c r="N263" s="5">
-        <v>72.52</v>
-      </c>
-      <c r="O263" s="5">
-        <v>73.17</v>
-      </c>
-      <c r="P263" s="5">
-        <v>73.930000000000007</v>
-      </c>
-      <c r="Q263" s="5">
-        <v>73.319999999999993</v>
-      </c>
-      <c r="R263" s="5">
-        <v>72.849999999999994</v>
-      </c>
-      <c r="S263" s="3"/>
+      <c r="M263" s="4">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="N263" s="4">
+        <v>72.5</v>
+      </c>
+      <c r="O263" s="4">
+        <v>73.2</v>
+      </c>
+      <c r="P263" s="4">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="Q263" s="4">
+        <v>73.3</v>
+      </c>
+      <c r="R263" s="4">
+        <v>72.8</v>
+      </c>
+      <c r="S263" s="4">
+        <v>76.3</v>
+      </c>
       <c r="T263" s="3"/>
       <c r="U263" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="264" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:21" ht="29.25">
       <c r="A264" s="2" t="s">
         <v>356</v>
       </c>
@@ -16474,13 +16595,15 @@
       <c r="R264" s="6">
         <v>84506</v>
       </c>
-      <c r="S264" s="3"/>
+      <c r="S264" s="6">
+        <v>295948</v>
+      </c>
       <c r="T264" s="3"/>
       <c r="U264" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="265" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:21" ht="29.25">
       <c r="A265" s="2" t="s">
         <v>356</v>
       </c>
@@ -16543,7 +16666,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="266" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:21" ht="29.25">
       <c r="A266" s="2" t="s">
         <v>372</v>
       </c>
@@ -16608,7 +16731,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="267" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:21" ht="29.25">
       <c r="A267" s="2" t="s">
         <v>372</v>
       </c>
@@ -16651,13 +16774,15 @@
         <v>74</v>
       </c>
       <c r="R267" s="3"/>
-      <c r="S267" s="3"/>
+      <c r="S267" s="6">
+        <v>63</v>
+      </c>
       <c r="T267" s="3"/>
       <c r="U267" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="268" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:21" ht="29.25">
       <c r="A268" s="2" t="s">
         <v>372</v>
       </c>
@@ -16692,33 +16817,35 @@
         <v>1.06</v>
       </c>
       <c r="L268" s="5">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="M268" s="5">
         <v>0.91</v>
       </c>
       <c r="N268" s="5">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="O268" s="5">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="P268" s="5">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="Q268" s="5">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="R268" s="5">
-        <v>0.84</v>
-      </c>
-      <c r="S268" s="3"/>
+        <v>0.83</v>
+      </c>
+      <c r="S268" s="5">
+        <v>0.72</v>
+      </c>
       <c r="T268" s="3"/>
       <c r="U268" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:21" ht="29.25">
       <c r="A269" s="2" t="s">
         <v>372</v>
       </c>
@@ -16779,7 +16906,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="270" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:21" ht="29.25">
       <c r="A270" s="2" t="s">
         <v>372</v>
       </c>
@@ -16840,7 +16967,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="271" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:21" ht="29.25">
       <c r="A271" s="2" t="s">
         <v>372</v>
       </c>
@@ -16901,7 +17028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="272" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:21" ht="29.25">
       <c r="A272" s="2" t="s">
         <v>372</v>
       </c>
@@ -16962,7 +17089,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="273" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" ht="29.25">
       <c r="A273" s="2" t="s">
         <v>372</v>
       </c>
@@ -17023,7 +17150,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="274" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" ht="29.25">
       <c r="A274" s="2" t="s">
         <v>372</v>
       </c>
@@ -17084,7 +17211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="275" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" ht="29.25">
       <c r="A275" s="2" t="s">
         <v>372</v>
       </c>
@@ -17145,7 +17272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" ht="29.25">
       <c r="A276" s="2" t="s">
         <v>372</v>
       </c>
@@ -17206,7 +17333,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="277" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" ht="29.25">
       <c r="A277" s="2" t="s">
         <v>372</v>
       </c>
@@ -17267,7 +17394,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="278" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" ht="29.25">
       <c r="A278" s="2" t="s">
         <v>372</v>
       </c>
@@ -17328,7 +17455,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="279" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" ht="29.25">
       <c r="A279" s="2" t="s">
         <v>372</v>
       </c>
@@ -17389,7 +17516,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="280" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" ht="29.25">
       <c r="A280" s="2" t="s">
         <v>372</v>
       </c>
@@ -17450,7 +17577,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="281" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" ht="29.25">
       <c r="A281" s="2" t="s">
         <v>372</v>
       </c>
@@ -17511,7 +17638,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="282" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" ht="29.25">
       <c r="A282" s="2" t="s">
         <v>372</v>
       </c>
@@ -17572,7 +17699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="283" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" ht="29.25">
       <c r="A283" s="2" t="s">
         <v>372</v>
       </c>
@@ -17633,7 +17760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="284" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" ht="29.25">
       <c r="A284" s="2" t="s">
         <v>372</v>
       </c>
@@ -17694,7 +17821,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="285" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" ht="29.25">
       <c r="A285" s="2" t="s">
         <v>372</v>
       </c>
@@ -17755,7 +17882,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="286" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" ht="29.25">
       <c r="A286" s="2" t="s">
         <v>372</v>
       </c>
@@ -17816,7 +17943,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="287" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" ht="29.25">
       <c r="A287" s="2" t="s">
         <v>372</v>
       </c>
@@ -17877,7 +18004,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="288" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" ht="29.25">
       <c r="A288" s="2" t="s">
         <v>372</v>
       </c>
@@ -17940,7 +18067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="289" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:21" ht="39">
       <c r="A289" s="2" t="s">
         <v>386</v>
       </c>
@@ -17996,14 +18123,14 @@
         <v>983.51</v>
       </c>
       <c r="S289" s="5">
-        <v>3378.18</v>
+        <v>3494.39</v>
       </c>
       <c r="T289" s="3"/>
       <c r="U289" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="290" spans="1:21" ht="36" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:21" ht="39">
       <c r="A290" s="2" t="s">
         <v>386</v>
       </c>
@@ -18059,14 +18186,14 @@
         <v>296.20999999999998</v>
       </c>
       <c r="S290" s="5">
-        <v>2558.85</v>
+        <v>2661.32</v>
       </c>
       <c r="T290" s="3"/>
       <c r="U290" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="291" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:21" ht="78">
       <c r="A291" s="2" t="s">
         <v>386</v>
       </c>
@@ -18129,7 +18256,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="292" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:21" ht="29.25">
       <c r="A292" s="2" t="s">
         <v>386</v>
       </c>
@@ -18186,7 +18313,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="293" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:21" ht="29.25">
       <c r="A293" s="2" t="s">
         <v>386</v>
       </c>
@@ -18243,7 +18370,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="294" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:21" ht="39">
       <c r="A294" s="2" t="s">
         <v>386</v>
       </c>
@@ -18292,7 +18419,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="295" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:21" ht="29.25">
       <c r="A295" s="2" t="s">
         <v>386</v>
       </c>
@@ -18349,7 +18476,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="296" spans="1:21" ht="27" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:21" ht="29.25">
       <c r="A296" s="2" t="s">
         <v>386</v>
       </c>
@@ -18404,25 +18531,65 @@
         <v>401</v>
       </c>
     </row>
-    <row r="297" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="10" t="s">
+    <row r="297" spans="1:21" ht="48.75">
+      <c r="A297" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B297" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B298" s="8"/>
+      <c r="C297" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D297" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E297" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F297" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G297" s="3"/>
+      <c r="H297" s="3"/>
+      <c r="I297" s="3"/>
+      <c r="J297" s="3"/>
+      <c r="K297" s="3"/>
+      <c r="L297" s="3"/>
+      <c r="M297" s="3"/>
+      <c r="N297" s="3"/>
+      <c r="O297" s="3"/>
+      <c r="P297" s="3"/>
+      <c r="Q297" s="3"/>
+      <c r="R297" s="3"/>
+      <c r="S297" s="3"/>
+      <c r="T297" s="6">
+        <v>114</v>
+      </c>
+      <c r="U297" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="298" spans="1:21" ht="0" hidden="1" customHeight="1"/>
+    <row r="299" spans="1:21" ht="18" customHeight="1"/>
+    <row r="300" spans="1:21" ht="17.100000000000001" customHeight="1">
+      <c r="A300" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="B300" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:C3"/>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A298:B298"/>
+    <mergeCell ref="A300:B300"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.39370078740157499"/>
-  <pageSetup paperSize="9" scale="62" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="63" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Okno serwisowe 06.02.2024 - aktualizacja excel
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -661,7 +661,7 @@
     <t>Promotion of stable forms of employment</t>
   </si>
   <si>
-    <t>8.4.a Percentage of paid employees in relation to the number of persons employed in national economy.</t>
+    <t>8.4.a Percentage of paid employees in relation to the number of persons employed in national economy</t>
   </si>
   <si>
     <t>Work activation of young people, women, persons aged 50+ , long-term unemployed as well as persons with disabilities</t>
@@ -1252,7 +1252,7 @@
     <t>The Ministry of Economic Development and Technology / The Chancellery of the  Prime Minister</t>
   </si>
   <si>
-    <t>Last update: 07-02-2024, 08:56</t>
+    <t>Last update: 09-02-2024, 11:15</t>
   </si>
 </sst>
 </file>
@@ -10650,7 +10650,9 @@
       <c r="R163" s="4">
         <v>80.400000000000006</v>
       </c>
-      <c r="S163" s="3"/>
+      <c r="S163" s="4">
+        <v>78.900000000000006</v>
+      </c>
       <c r="T163" s="3"/>
       <c r="U163" s="2" t="s">
         <v>28</v>
@@ -10711,7 +10713,9 @@
       <c r="R164" s="4">
         <v>84.2</v>
       </c>
-      <c r="S164" s="3"/>
+      <c r="S164" s="4">
+        <v>83.1</v>
+      </c>
       <c r="T164" s="3"/>
       <c r="U164" s="2" t="s">
         <v>28</v>
@@ -10772,7 +10776,9 @@
       <c r="R165" s="4">
         <v>77.099999999999994</v>
       </c>
-      <c r="S165" s="3"/>
+      <c r="S165" s="4">
+        <v>75.2</v>
+      </c>
       <c r="T165" s="3"/>
       <c r="U165" s="2" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Okno 16.07.2024 - aktualizacja EXCEL
</commit_message>
<xml_diff>
--- a/assets/excel/en/national_sdg_indicators.xlsx
+++ b/assets/excel/en/national_sdg_indicators.xlsx
@@ -1249,7 +1249,7 @@
     <t>The Ministry of Economic Development and Technology / The Chancellery of the  Prime Minister</t>
   </si>
   <si>
-    <t>Last update: 17-07-2024, 07:48</t>
+    <t>Last update: 18-07-2024, 09:22</t>
   </si>
 </sst>
 </file>
@@ -2042,7 +2042,7 @@
         <v>13.9</v>
       </c>
       <c r="N6" s="4">
-        <v>16</v>
+        <v>15.9</v>
       </c>
       <c r="O6" s="4">
         <v>19.3</v>
@@ -8347,7 +8347,7 @@
         <v>13.9</v>
       </c>
       <c r="N125" s="4">
-        <v>16</v>
+        <v>15.9</v>
       </c>
       <c r="O125" s="4">
         <v>19.3</v>

</xml_diff>